<commit_message>
%48.5 DEL EXCEL WAAAAAAAAA :p
</commit_message>
<xml_diff>
--- a/Consigna/correcciones20162C.xlsx
+++ b/Consigna/correcciones20162C.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pablo\UNLAM\2016\TP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\PrograWeb3-AlquilaCocheras\Consigna\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$F$180</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="151">
   <si>
     <t xml:space="preserve">Página de inicio​ (​/default.aspx​)  </t>
   </si>
@@ -646,6 +646,15 @@
   </si>
   <si>
     <t>Enviaron este excel marcando en Correccion, con B lo que pudieron hacer?</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>FF</t>
   </si>
 </sst>
 </file>
@@ -794,6 +803,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -801,15 +819,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2181,7 +2190,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2256,6 +2265,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2291,6 +2317,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2446,13 +2489,13 @@
   <dimension ref="A1:O181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B176" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D180" sqref="D180"/>
+      <selection pane="bottomRight" activeCell="H181" sqref="H181"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.42578125" style="2" customWidth="1"/>
@@ -2496,14 +2539,14 @@
       </c>
       <c r="K1">
         <f>COUNTIF(F:F, "B")</f>
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>146</v>
       </c>
       <c r="M1" s="14">
         <f>K1/I1</f>
-        <v>0</v>
+        <v>0.48920863309352519</v>
       </c>
       <c r="N1" s="13" t="s">
         <v>137</v>
@@ -2517,15 +2560,15 @@
       <c r="A2" s="11">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20"/>
     </row>
     <row r="3" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -2537,6 +2580,9 @@
       <c r="E3" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F3" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
@@ -2548,6 +2594,9 @@
       <c r="E4" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F4" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="5" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
@@ -2565,25 +2614,25 @@
       <c r="A6" s="11">
         <v>1</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="17"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="20"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="17"/>
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2592,6 +2641,9 @@
       </c>
       <c r="E8" s="5" t="s">
         <v>15</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -2603,6 +2655,9 @@
       <c r="E9" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F9" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
@@ -2613,6 +2668,9 @@
       <c r="E10" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F10" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="11" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="D11" s="5" t="s">
@@ -2629,15 +2687,18 @@
       <c r="E12" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F12" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="20"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D14" s="5" t="s">
@@ -2649,12 +2710,12 @@
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8"/>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="20"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="17"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D16" s="5" t="s">
@@ -2664,7 +2725,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="5" t="s">
         <v>132</v>
       </c>
@@ -2672,7 +2733,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D18" s="5" t="s">
         <v>13</v>
       </c>
@@ -2680,7 +2741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D19" s="5" t="s">
         <v>14</v>
       </c>
@@ -2688,7 +2749,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="D20" s="5" t="s">
         <v>17</v>
       </c>
@@ -2696,7 +2757,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="D21" s="5" t="s">
         <v>18</v>
       </c>
@@ -2704,118 +2765,148 @@
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>2</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="17"/>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="20"/>
+    </row>
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D23" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D24" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F24" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D25" s="5" t="s">
         <v>22</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D26" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F26" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D27" s="5" t="s">
         <v>133</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F27" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D28" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F28" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D29" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F29" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="20"/>
-    </row>
-    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D30" s="17"/>
+    </row>
+    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="D31" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="D32" s="9" t="s">
         <v>34</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>3</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="17"/>
-    </row>
-    <row r="34" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="20"/>
+    </row>
+    <row r="34" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D34" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F34" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="4" t="s">
@@ -2824,8 +2915,11 @@
       <c r="E35" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="4" t="s">
@@ -2834,33 +2928,42 @@
       <c r="E36" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F36" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D37" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F37" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D38" s="5" t="s">
         <v>26</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H38" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B39" s="8"/>
-      <c r="C39" s="18" t="s">
+      <c r="C39" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="20"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="17"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B40" s="8"/>
       <c r="C40" s="7"/>
       <c r="D40" s="5" t="s">
@@ -2869,8 +2972,11 @@
       <c r="E40" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H40" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="8"/>
       <c r="C41" s="7"/>
       <c r="D41" s="5" t="s">
@@ -2879,8 +2985,11 @@
       <c r="E41" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H41" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B42" s="8"/>
       <c r="C42" s="7"/>
       <c r="D42" s="5" t="s">
@@ -2889,8 +2998,11 @@
       <c r="E42" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H42" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B43" s="8"/>
       <c r="C43" s="7"/>
       <c r="D43" s="5" t="s">
@@ -2899,8 +3011,11 @@
       <c r="E43" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="F43" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B44" s="8"/>
       <c r="C44" s="7"/>
       <c r="D44" s="5" t="s">
@@ -2909,24 +3024,33 @@
       <c r="E44" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H44" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D45" s="5" t="s">
         <v>29</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F45" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D46" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F46" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B47" s="8"/>
       <c r="C47" s="7"/>
       <c r="D47" s="5" t="s">
@@ -2935,17 +3059,20 @@
       <c r="E47" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I47" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48" s="8"/>
-      <c r="C48" s="18" t="s">
+      <c r="C48" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="20"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="17"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
       <c r="C49" s="7"/>
       <c r="D49" s="5" t="s">
@@ -2954,8 +3081,11 @@
       <c r="E49" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F49" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="8"/>
       <c r="C50" s="7"/>
       <c r="D50" s="5" t="s">
@@ -2964,38 +3094,47 @@
       <c r="E50" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F50" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D51" s="5" t="s">
         <v>39</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F51" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="11">
         <v>4</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B52" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16" t="s">
+      <c r="C52" s="19"/>
+      <c r="D52" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E52" s="16"/>
-      <c r="F52" s="17"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E52" s="19"/>
+      <c r="F52" s="20"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D53" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F53" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="4" t="s">
@@ -3004,8 +3143,11 @@
       <c r="E54" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F54" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
       <c r="D55" s="4" t="s">
@@ -3014,48 +3156,63 @@
       <c r="E55" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="F55" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="D56" s="5" t="s">
         <v>41</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C57" s="18" t="s">
+      <c r="I56" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C57" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="20"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D57" s="16"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="17"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D58" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F58" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D59" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F59" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D60" s="5" t="s">
         <v>44</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F60" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D61" s="5" t="s">
         <v>45</v>
       </c>
@@ -3063,45 +3220,51 @@
         <v>131</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C62" s="18" t="s">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C62" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D62" s="19"/>
-      <c r="E62" s="19"/>
-      <c r="F62" s="20"/>
-    </row>
-    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="17"/>
+    </row>
+    <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D63" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H63" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="11">
         <v>5</v>
       </c>
-      <c r="B64" s="15" t="s">
+      <c r="B64" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C64" s="16" t="s">
+      <c r="C64" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="17"/>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D64" s="19"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="20"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D65" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="66" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F65" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
       <c r="D66" s="4" t="s">
@@ -3110,8 +3273,11 @@
       <c r="E66" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F66" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
       <c r="D67" s="4" t="s">
@@ -3120,72 +3286,96 @@
       <c r="E67" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="68" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F67" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D68" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E68" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C69" s="18" t="s">
+      <c r="H68" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C69" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D69" s="19"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="20"/>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D69" s="16"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="17"/>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D70" s="5" t="s">
         <v>48</v>
       </c>
       <c r="E70" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="71" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F70" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D71" s="5" t="s">
         <v>51</v>
       </c>
       <c r="E71" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F71" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D72" s="5" t="s">
         <v>52</v>
       </c>
       <c r="E72" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H72" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D73" s="5" t="s">
         <v>67</v>
       </c>
       <c r="E73" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H73" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D74" s="5" t="s">
         <v>68</v>
       </c>
       <c r="E74" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F74" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D75" s="5" t="s">
         <v>69</v>
       </c>
       <c r="E75" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H75" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D76" s="5" t="s">
         <v>70</v>
       </c>
@@ -3193,181 +3383,241 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D77" s="5" t="s">
         <v>56</v>
       </c>
       <c r="E77" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F77" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D78" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E78" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H78" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D79" s="5" t="s">
         <v>72</v>
       </c>
       <c r="E79" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F79" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D80" s="5" t="s">
         <v>71</v>
       </c>
       <c r="E80" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H80" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D81" s="5" t="s">
         <v>54</v>
       </c>
       <c r="E81" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F81" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D82" s="5" t="s">
         <v>55</v>
       </c>
       <c r="E82" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F82" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D83" s="5" t="s">
         <v>57</v>
       </c>
       <c r="E83" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H83" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D84" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E84" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F84" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D85" s="5" t="s">
         <v>59</v>
       </c>
       <c r="E85" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H85" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D86" s="5" t="s">
         <v>60</v>
       </c>
       <c r="E86" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F86" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D87" s="5" t="s">
         <v>61</v>
       </c>
       <c r="E87" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F87" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D88" s="5" t="s">
         <v>74</v>
       </c>
       <c r="E88" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F88" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D89" s="5" t="s">
         <v>62</v>
       </c>
       <c r="E89" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I89" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D90" s="5" t="s">
         <v>63</v>
       </c>
       <c r="E90" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F90" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D91" s="5" t="s">
         <v>64</v>
       </c>
       <c r="E91" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H91" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D92" s="5" t="s">
         <v>73</v>
       </c>
       <c r="E92" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F92" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="H92" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D93" s="5" t="s">
         <v>65</v>
       </c>
       <c r="E93" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C94" s="18" t="s">
+      <c r="F93" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C94" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D94" s="19"/>
-      <c r="E94" s="19"/>
-      <c r="F94" s="20"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D94" s="16"/>
+      <c r="E94" s="16"/>
+      <c r="F94" s="17"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D95" s="5" t="s">
         <v>66</v>
       </c>
       <c r="E95" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H95" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="11">
         <v>6</v>
       </c>
-      <c r="B96" s="15" t="s">
+      <c r="B96" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C96" s="16" t="s">
+      <c r="C96" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="D96" s="16"/>
-      <c r="E96" s="16"/>
-      <c r="F96" s="17"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D96" s="19"/>
+      <c r="E96" s="19"/>
+      <c r="F96" s="20"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D97" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E97" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F97" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
       <c r="D98" s="4" t="s">
@@ -3376,8 +3626,11 @@
       <c r="E98" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F98" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B99" s="6"/>
       <c r="C99" s="6"/>
       <c r="D99" s="4" t="s">
@@ -3386,32 +3639,41 @@
       <c r="E99" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F99" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D100" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E100" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C101" s="18" t="s">
+      <c r="F100" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C101" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D101" s="19"/>
-      <c r="E101" s="19"/>
-      <c r="F101" s="20"/>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D101" s="16"/>
+      <c r="E101" s="16"/>
+      <c r="F101" s="17"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D102" s="5" t="s">
         <v>76</v>
       </c>
       <c r="E102" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F102" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C103" s="8"/>
       <c r="D103" s="9" t="s">
         <v>77</v>
@@ -3419,8 +3681,11 @@
       <c r="E103" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F103" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C104" s="8"/>
       <c r="D104" s="9" t="s">
         <v>80</v>
@@ -3428,70 +3693,88 @@
       <c r="E104" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F104" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D105" s="5" t="s">
         <v>78</v>
       </c>
       <c r="E105" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F105" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D106" s="5" t="s">
         <v>81</v>
       </c>
       <c r="E106" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="F106" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="D107" s="5" t="s">
         <v>79</v>
       </c>
       <c r="E107" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C108" s="18" t="s">
+      <c r="I107" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C108" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D108" s="19"/>
-      <c r="E108" s="19"/>
-      <c r="F108" s="20"/>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D108" s="16"/>
+      <c r="E108" s="16"/>
+      <c r="F108" s="17"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D109" s="5" t="s">
         <v>66</v>
       </c>
       <c r="E109" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I109" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="11">
         <v>7</v>
       </c>
-      <c r="B110" s="15" t="s">
+      <c r="B110" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C110" s="16" t="s">
+      <c r="C110" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="D110" s="16"/>
-      <c r="E110" s="16"/>
-      <c r="F110" s="17"/>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D110" s="19"/>
+      <c r="E110" s="19"/>
+      <c r="F110" s="20"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D111" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E111" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F111" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="6"/>
       <c r="C112" s="6"/>
       <c r="D112" s="4" t="s">
@@ -3500,8 +3783,11 @@
       <c r="E112" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F112" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
       <c r="D113" s="4" t="s">
@@ -3510,32 +3796,41 @@
       <c r="E113" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+      <c r="F113" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="D114" s="5" t="s">
         <v>134</v>
       </c>
       <c r="E114" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F114" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="D115" s="5" t="s">
         <v>88</v>
       </c>
       <c r="E115" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C116" s="18" t="s">
+      <c r="I115" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C116" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D116" s="19"/>
-      <c r="E116" s="19"/>
-      <c r="F116" s="20"/>
-    </row>
-    <row r="117" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D116" s="16"/>
+      <c r="E116" s="16"/>
+      <c r="F116" s="17"/>
+    </row>
+    <row r="117" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C117" s="7"/>
       <c r="D117" s="5" t="s">
         <v>84</v>
@@ -3543,8 +3838,11 @@
       <c r="E117" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H117" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C118" s="7"/>
       <c r="D118" s="5" t="s">
         <v>85</v>
@@ -3552,54 +3850,66 @@
       <c r="E118" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H118" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="D119" s="5" t="s">
         <v>83</v>
       </c>
       <c r="E119" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C120" s="18" t="s">
+      <c r="J119" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C120" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D120" s="19"/>
-      <c r="E120" s="19"/>
-      <c r="F120" s="20"/>
-    </row>
-    <row r="121" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D120" s="16"/>
+      <c r="E120" s="16"/>
+      <c r="F120" s="17"/>
+    </row>
+    <row r="121" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="D121" s="5" t="s">
         <v>86</v>
       </c>
       <c r="E121" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J121" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="11">
         <v>8</v>
       </c>
-      <c r="B122" s="15" t="s">
+      <c r="B122" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="C122" s="16" t="s">
+      <c r="C122" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D122" s="16"/>
-      <c r="E122" s="16"/>
-      <c r="F122" s="17"/>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D122" s="19"/>
+      <c r="E122" s="19"/>
+      <c r="F122" s="20"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D123" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E123" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F123" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" s="6"/>
       <c r="C124" s="6"/>
       <c r="D124" s="4" t="s">
@@ -3608,8 +3918,11 @@
       <c r="E124" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F124" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B125" s="6"/>
       <c r="C125" s="6"/>
       <c r="D125" s="4" t="s">
@@ -3618,32 +3931,41 @@
       <c r="E125" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="F125" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="D126" s="5" t="s">
         <v>90</v>
       </c>
       <c r="E126" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H126" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D127" s="5" t="s">
         <v>89</v>
       </c>
       <c r="E127" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C128" s="18" t="s">
+      <c r="F127" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C128" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D128" s="19"/>
-      <c r="E128" s="19"/>
-      <c r="F128" s="20"/>
-    </row>
-    <row r="129" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D128" s="16"/>
+      <c r="E128" s="16"/>
+      <c r="F128" s="17"/>
+    </row>
+    <row r="129" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="C129" s="7"/>
       <c r="D129" s="5" t="s">
         <v>135</v>
@@ -3651,30 +3973,36 @@
       <c r="E129" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H129" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="11">
         <v>8.1</v>
       </c>
-      <c r="B130" s="15" t="s">
+      <c r="B130" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="C130" s="16" t="s">
+      <c r="C130" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="D130" s="16"/>
-      <c r="E130" s="16"/>
-      <c r="F130" s="17"/>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D130" s="19"/>
+      <c r="E130" s="19"/>
+      <c r="F130" s="20"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D131" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E131" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H131" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="6"/>
       <c r="C132" s="6"/>
       <c r="D132" s="4" t="s">
@@ -3683,8 +4011,11 @@
       <c r="E132" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H132" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B133" s="6"/>
       <c r="C133" s="6"/>
       <c r="D133" s="4" t="s">
@@ -3693,94 +4024,127 @@
       <c r="E133" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="H133" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="D134" s="5" t="s">
         <v>92</v>
       </c>
       <c r="E134" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H134" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D135" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E135" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H135" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D136" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E136" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H136" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D137" s="5" t="s">
         <v>94</v>
       </c>
       <c r="E137" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H137" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D138" s="5" t="s">
         <v>95</v>
       </c>
       <c r="E138" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H138" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D139" s="5" t="s">
         <v>99</v>
       </c>
       <c r="E139" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H139" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D140" s="5" t="s">
         <v>98</v>
       </c>
       <c r="E140" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H140" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D141" s="5" t="s">
         <v>96</v>
       </c>
       <c r="E141" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H141" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D142" s="5" t="s">
         <v>97</v>
       </c>
       <c r="E142" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="H142" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="D143" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E143" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C144" s="18" t="s">
+      <c r="H143" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C144" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D144" s="19"/>
-      <c r="E144" s="19"/>
-      <c r="F144" s="20"/>
+      <c r="D144" s="16"/>
+      <c r="E144" s="16"/>
+      <c r="F144" s="17"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D145" s="5" t="s">
@@ -3855,12 +4219,12 @@
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C154" s="18" t="s">
+      <c r="C154" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D154" s="19"/>
-      <c r="E154" s="19"/>
-      <c r="F154" s="20"/>
+      <c r="D154" s="16"/>
+      <c r="E154" s="16"/>
+      <c r="F154" s="17"/>
     </row>
     <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D155" s="5" t="s">
@@ -3882,15 +4246,15 @@
       <c r="A157" s="11">
         <v>9</v>
       </c>
-      <c r="B157" s="15" t="s">
+      <c r="B157" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C157" s="16" t="s">
+      <c r="C157" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="D157" s="16"/>
-      <c r="E157" s="16"/>
-      <c r="F157" s="17"/>
+      <c r="D157" s="19"/>
+      <c r="E157" s="19"/>
+      <c r="F157" s="20"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D158" s="4" t="s">
@@ -3972,15 +4336,15 @@
       <c r="A167" s="11">
         <v>10</v>
       </c>
-      <c r="B167" s="15" t="s">
+      <c r="B167" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C167" s="16" t="s">
+      <c r="C167" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="D167" s="16"/>
-      <c r="E167" s="16"/>
-      <c r="F167" s="17"/>
+      <c r="D167" s="19"/>
+      <c r="E167" s="19"/>
+      <c r="F167" s="20"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D168" s="4" t="s">
@@ -4054,72 +4418,73 @@
       <c r="A176" s="11">
         <v>11</v>
       </c>
-      <c r="B176" s="15" t="s">
+      <c r="B176" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="C176" s="16" t="s">
+      <c r="C176" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="D176" s="16"/>
-      <c r="E176" s="16"/>
-      <c r="F176" s="17"/>
-    </row>
-    <row r="177" spans="4:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D176" s="19"/>
+      <c r="E176" s="19"/>
+      <c r="F176" s="20"/>
+    </row>
+    <row r="177" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D177" s="5" t="s">
         <v>120</v>
       </c>
       <c r="E177" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="178" spans="4:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F177" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="178" spans="4:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D178" s="5" t="s">
         <v>121</v>
       </c>
       <c r="E178" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="179" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F178" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="179" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D179" s="5" t="s">
         <v>122</v>
       </c>
       <c r="E179" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="180" spans="4:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="F179" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="180" spans="4:6" ht="75" x14ac:dyDescent="0.25">
       <c r="D180" s="5" t="s">
         <v>123</v>
       </c>
       <c r="E180" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="181" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F180" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="181" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D181" s="5" t="s">
         <v>147</v>
       </c>
       <c r="E181" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F181" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C62:F62"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C154:F154"/>
-    <mergeCell ref="B167:F167"/>
-    <mergeCell ref="B176:F176"/>
-    <mergeCell ref="B157:F157"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C69:F69"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="C108:F108"/>
-    <mergeCell ref="C116:F116"/>
-    <mergeCell ref="C120:F120"/>
-    <mergeCell ref="C128:F128"/>
-    <mergeCell ref="C144:F144"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B22:F22"/>
@@ -4136,6 +4501,20 @@
     <mergeCell ref="C39:F39"/>
     <mergeCell ref="C48:F48"/>
     <mergeCell ref="C57:F57"/>
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C154:F154"/>
+    <mergeCell ref="B167:F167"/>
+    <mergeCell ref="B176:F176"/>
+    <mergeCell ref="B157:F157"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C69:F69"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="C108:F108"/>
+    <mergeCell ref="C116:F116"/>
+    <mergeCell ref="C120:F120"/>
+    <mergeCell ref="C128:F128"/>
+    <mergeCell ref="C144:F144"/>
   </mergeCells>
   <conditionalFormatting sqref="E16:E21 E149:E153 E1 E11:E12 E37:E38 E56 E100 E161:E166 E171:E175 E14 E23:E32 E40:E47 E63 E49:E51 E58:E61 E68 E81:E93 E70:E78 E102:E107 E117:E119 E121 E129 E95 E109 E114:E115 E134:E143 E155:E156 E3:E5 E126:E127 E177:E1048576">
     <cfRule type="cellIs" dxfId="134" priority="140" operator="equal">
@@ -4845,7 +5224,7 @@
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
ultimo commit antes de la entrega
</commit_message>
<xml_diff>
--- a/Consigna/correcciones20162C.xlsx
+++ b/Consigna/correcciones20162C.xlsx
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="149">
   <si>
     <t xml:space="preserve">Página de inicio​ (​/default.aspx​)  </t>
   </si>
@@ -648,13 +648,7 @@
     <t>Enviaron este excel marcando en Correccion, con B lo que pudieron hacer?</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>FF</t>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -2489,10 +2483,10 @@
   <dimension ref="A1:O181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B172" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H181" sqref="H181"/>
+      <selection pane="bottomRight" activeCell="D179" sqref="D179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2539,14 +2533,14 @@
       </c>
       <c r="K1">
         <f>COUNTIF(F:F, "B")</f>
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>146</v>
       </c>
       <c r="M1" s="14">
         <f>K1/I1</f>
-        <v>0.48920863309352519</v>
+        <v>0.66187050359712229</v>
       </c>
       <c r="N1" s="13" t="s">
         <v>137</v>
@@ -2725,7 +2719,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="5" t="s">
         <v>132</v>
       </c>
@@ -2733,7 +2727,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D18" s="5" t="s">
         <v>13</v>
       </c>
@@ -2741,7 +2735,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D19" s="5" t="s">
         <v>14</v>
       </c>
@@ -2749,7 +2743,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="D20" s="5" t="s">
         <v>17</v>
       </c>
@@ -2757,7 +2751,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="D21" s="5" t="s">
         <v>18</v>
       </c>
@@ -2765,7 +2759,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>2</v>
       </c>
@@ -2777,7 +2771,7 @@
       <c r="E22" s="19"/>
       <c r="F22" s="20"/>
     </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D23" s="5" t="s">
         <v>20</v>
       </c>
@@ -2788,7 +2782,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D24" s="5" t="s">
         <v>21</v>
       </c>
@@ -2799,7 +2793,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D25" s="5" t="s">
         <v>22</v>
       </c>
@@ -2810,7 +2804,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D26" s="5" t="s">
         <v>23</v>
       </c>
@@ -2821,7 +2815,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D27" s="5" t="s">
         <v>133</v>
       </c>
@@ -2832,7 +2826,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D28" s="5" t="s">
         <v>31</v>
       </c>
@@ -2843,7 +2837,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D29" s="5" t="s">
         <v>33</v>
       </c>
@@ -2854,36 +2848,36 @@
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
       <c r="C30" s="15" t="s">
         <v>28</v>
       </c>
       <c r="D30" s="17"/>
     </row>
-    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="D31" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H31" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="F31" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="D32" s="9" t="s">
         <v>34</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H32" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F32" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>3</v>
       </c>
@@ -2895,7 +2889,7 @@
       <c r="E33" s="19"/>
       <c r="F33" s="20"/>
     </row>
-    <row r="34" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D34" s="4" t="s">
         <v>1</v>
       </c>
@@ -2906,7 +2900,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="4" t="s">
@@ -2919,7 +2913,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="4" t="s">
@@ -2932,7 +2926,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="D37" s="5" t="s">
         <v>27</v>
       </c>
@@ -2943,18 +2937,18 @@
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D38" s="5" t="s">
         <v>26</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H38" t="s">
+      <c r="F38" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" s="8"/>
       <c r="C39" s="15" t="s">
         <v>28</v>
@@ -2963,7 +2957,7 @@
       <c r="E39" s="16"/>
       <c r="F39" s="17"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" s="8"/>
       <c r="C40" s="7"/>
       <c r="D40" s="5" t="s">
@@ -2972,11 +2966,11 @@
       <c r="E40" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H40" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F40" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="8"/>
       <c r="C41" s="7"/>
       <c r="D41" s="5" t="s">
@@ -2985,11 +2979,11 @@
       <c r="E41" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H41" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="F41" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B42" s="8"/>
       <c r="C42" s="7"/>
       <c r="D42" s="5" t="s">
@@ -2998,11 +2992,8 @@
       <c r="E42" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H42" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" s="8"/>
       <c r="C43" s="7"/>
       <c r="D43" s="5" t="s">
@@ -3015,7 +3006,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B44" s="8"/>
       <c r="C44" s="7"/>
       <c r="D44" s="5" t="s">
@@ -3024,11 +3015,8 @@
       <c r="E44" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H44" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D45" s="5" t="s">
         <v>29</v>
       </c>
@@ -3039,7 +3027,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D46" s="5" t="s">
         <v>30</v>
       </c>
@@ -3050,7 +3038,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B47" s="8"/>
       <c r="C47" s="7"/>
       <c r="D47" s="5" t="s">
@@ -3059,11 +3047,8 @@
       <c r="E47" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I47" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" s="8"/>
       <c r="C48" s="15" t="s">
         <v>6</v>
@@ -3072,7 +3057,7 @@
       <c r="E48" s="16"/>
       <c r="F48" s="17"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
       <c r="C49" s="7"/>
       <c r="D49" s="5" t="s">
@@ -3085,7 +3070,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="8"/>
       <c r="C50" s="7"/>
       <c r="D50" s="5" t="s">
@@ -3098,7 +3083,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D51" s="5" t="s">
         <v>39</v>
       </c>
@@ -3109,7 +3094,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="11">
         <v>4</v>
       </c>
@@ -3123,7 +3108,7 @@
       <c r="E52" s="19"/>
       <c r="F52" s="20"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D53" s="4" t="s">
         <v>1</v>
       </c>
@@ -3134,7 +3119,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="4" t="s">
@@ -3147,7 +3132,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
       <c r="D55" s="4" t="s">
@@ -3160,18 +3145,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="D56" s="5" t="s">
         <v>41</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I56" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C57" s="15" t="s">
         <v>6</v>
       </c>
@@ -3179,7 +3161,7 @@
       <c r="E57" s="16"/>
       <c r="F57" s="17"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D58" s="5" t="s">
         <v>42</v>
       </c>
@@ -3190,7 +3172,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D59" s="5" t="s">
         <v>43</v>
       </c>
@@ -3201,7 +3183,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D60" s="5" t="s">
         <v>44</v>
       </c>
@@ -3212,7 +3194,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="D61" s="5" t="s">
         <v>45</v>
       </c>
@@ -3220,7 +3202,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C62" s="15" t="s">
         <v>10</v>
       </c>
@@ -3228,18 +3210,15 @@
       <c r="E62" s="16"/>
       <c r="F62" s="17"/>
     </row>
-    <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D63" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H63" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="11">
         <v>5</v>
       </c>
@@ -3253,7 +3232,7 @@
       <c r="E64" s="19"/>
       <c r="F64" s="20"/>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D65" s="4" t="s">
         <v>1</v>
       </c>
@@ -3264,7 +3243,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="66" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
       <c r="D66" s="4" t="s">
@@ -3277,7 +3256,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
       <c r="D67" s="4" t="s">
@@ -3290,18 +3269,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="68" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D68" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E68" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H68" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C69" s="15" t="s">
         <v>6</v>
       </c>
@@ -3309,7 +3285,7 @@
       <c r="E69" s="16"/>
       <c r="F69" s="17"/>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D70" s="5" t="s">
         <v>48</v>
       </c>
@@ -3320,7 +3296,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D71" s="5" t="s">
         <v>51</v>
       </c>
@@ -3331,29 +3307,29 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D72" s="5" t="s">
         <v>52</v>
       </c>
       <c r="E72" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H72" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F72" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D73" s="5" t="s">
         <v>67</v>
       </c>
       <c r="E73" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H73" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F73" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D74" s="5" t="s">
         <v>68</v>
       </c>
@@ -3364,26 +3340,29 @@
         <v>139</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D75" s="5" t="s">
         <v>69</v>
       </c>
       <c r="E75" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H75" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F75" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D76" s="5" t="s">
         <v>70</v>
       </c>
       <c r="E76" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F76" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D77" s="5" t="s">
         <v>56</v>
       </c>
@@ -3394,18 +3373,18 @@
         <v>139</v>
       </c>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D78" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E78" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H78" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F78" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D79" s="5" t="s">
         <v>72</v>
       </c>
@@ -3416,18 +3395,18 @@
         <v>139</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D80" s="5" t="s">
         <v>71</v>
       </c>
       <c r="E80" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H80" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F80" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D81" s="5" t="s">
         <v>54</v>
       </c>
@@ -3438,7 +3417,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D82" s="5" t="s">
         <v>55</v>
       </c>
@@ -3449,18 +3428,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D83" s="5" t="s">
         <v>57</v>
       </c>
       <c r="E83" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H83" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D84" s="5" t="s">
         <v>58</v>
       </c>
@@ -3471,18 +3447,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D85" s="5" t="s">
         <v>59</v>
       </c>
       <c r="E85" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H85" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D86" s="5" t="s">
         <v>60</v>
       </c>
@@ -3493,7 +3466,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D87" s="5" t="s">
         <v>61</v>
       </c>
@@ -3504,7 +3477,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D88" s="5" t="s">
         <v>74</v>
       </c>
@@ -3515,18 +3488,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D89" s="5" t="s">
         <v>62</v>
       </c>
       <c r="E89" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I89" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D90" s="5" t="s">
         <v>63</v>
       </c>
@@ -3537,18 +3507,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D91" s="5" t="s">
         <v>64</v>
       </c>
       <c r="E91" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H91" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D92" s="5" t="s">
         <v>73</v>
       </c>
@@ -3558,11 +3525,8 @@
       <c r="F92" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="H92" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D93" s="5" t="s">
         <v>65</v>
       </c>
@@ -3573,7 +3537,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C94" s="15" t="s">
         <v>10</v>
       </c>
@@ -3581,18 +3545,15 @@
       <c r="E94" s="16"/>
       <c r="F94" s="17"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D95" s="5" t="s">
         <v>66</v>
       </c>
       <c r="E95" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H95" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="11">
         <v>6</v>
       </c>
@@ -3606,7 +3567,7 @@
       <c r="E96" s="19"/>
       <c r="F96" s="20"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D97" s="4" t="s">
         <v>1</v>
       </c>
@@ -3617,7 +3578,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
       <c r="D98" s="4" t="s">
@@ -3630,7 +3591,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B99" s="6"/>
       <c r="C99" s="6"/>
       <c r="D99" s="4" t="s">
@@ -3643,7 +3604,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D100" s="5" t="s">
         <v>11</v>
       </c>
@@ -3654,7 +3615,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C101" s="15" t="s">
         <v>6</v>
       </c>
@@ -3662,7 +3623,7 @@
       <c r="E101" s="16"/>
       <c r="F101" s="17"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D102" s="5" t="s">
         <v>76</v>
       </c>
@@ -3673,7 +3634,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C103" s="8"/>
       <c r="D103" s="9" t="s">
         <v>77</v>
@@ -3685,7 +3646,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C104" s="8"/>
       <c r="D104" s="9" t="s">
         <v>80</v>
@@ -3697,7 +3658,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D105" s="5" t="s">
         <v>78</v>
       </c>
@@ -3708,7 +3669,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D106" s="5" t="s">
         <v>81</v>
       </c>
@@ -3719,18 +3680,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="D107" s="5" t="s">
         <v>79</v>
       </c>
       <c r="E107" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I107" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C108" s="15" t="s">
         <v>10</v>
       </c>
@@ -3738,18 +3696,15 @@
       <c r="E108" s="16"/>
       <c r="F108" s="17"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D109" s="5" t="s">
         <v>66</v>
       </c>
       <c r="E109" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I109" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="11">
         <v>7</v>
       </c>
@@ -3763,7 +3718,7 @@
       <c r="E110" s="19"/>
       <c r="F110" s="20"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D111" s="4" t="s">
         <v>1</v>
       </c>
@@ -3774,7 +3729,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="6"/>
       <c r="C112" s="6"/>
       <c r="D112" s="4" t="s">
@@ -3787,7 +3742,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
       <c r="D113" s="4" t="s">
@@ -3800,7 +3755,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="D114" s="5" t="s">
         <v>134</v>
       </c>
@@ -3811,18 +3766,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D115" s="5" t="s">
         <v>88</v>
       </c>
       <c r="E115" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I115" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C116" s="15" t="s">
         <v>6</v>
       </c>
@@ -3830,7 +3782,7 @@
       <c r="E116" s="16"/>
       <c r="F116" s="17"/>
     </row>
-    <row r="117" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C117" s="7"/>
       <c r="D117" s="5" t="s">
         <v>84</v>
@@ -3838,11 +3790,8 @@
       <c r="E117" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H117" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C118" s="7"/>
       <c r="D118" s="5" t="s">
         <v>85</v>
@@ -3850,22 +3799,16 @@
       <c r="E118" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H118" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="D119" s="5" t="s">
         <v>83</v>
       </c>
       <c r="E119" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J119" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C120" s="15" t="s">
         <v>10</v>
       </c>
@@ -3873,18 +3816,15 @@
       <c r="E120" s="16"/>
       <c r="F120" s="17"/>
     </row>
-    <row r="121" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D121" s="5" t="s">
         <v>86</v>
       </c>
       <c r="E121" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J121" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="11">
         <v>8</v>
       </c>
@@ -3898,7 +3838,7 @@
       <c r="E122" s="19"/>
       <c r="F122" s="20"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D123" s="4" t="s">
         <v>1</v>
       </c>
@@ -3909,7 +3849,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="124" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" s="6"/>
       <c r="C124" s="6"/>
       <c r="D124" s="4" t="s">
@@ -3922,7 +3862,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B125" s="6"/>
       <c r="C125" s="6"/>
       <c r="D125" s="4" t="s">
@@ -3935,18 +3875,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="126" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="D126" s="5" t="s">
         <v>90</v>
       </c>
       <c r="E126" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H126" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D127" s="5" t="s">
         <v>89</v>
       </c>
@@ -3957,7 +3894,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C128" s="15" t="s">
         <v>10</v>
       </c>
@@ -3965,7 +3902,7 @@
       <c r="E128" s="16"/>
       <c r="F128" s="17"/>
     </row>
-    <row r="129" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="C129" s="7"/>
       <c r="D129" s="5" t="s">
         <v>135</v>
@@ -3973,11 +3910,11 @@
       <c r="E129" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H129" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F129" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="11">
         <v>8.1</v>
       </c>
@@ -3991,18 +3928,18 @@
       <c r="E130" s="19"/>
       <c r="F130" s="20"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D131" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E131" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H131" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F131" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="6"/>
       <c r="C132" s="6"/>
       <c r="D132" s="4" t="s">
@@ -4011,11 +3948,11 @@
       <c r="E132" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H132" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F132" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B133" s="6"/>
       <c r="C133" s="6"/>
       <c r="D133" s="4" t="s">
@@ -4024,121 +3961,109 @@
       <c r="E133" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H133" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="F133" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="D134" s="5" t="s">
         <v>92</v>
       </c>
       <c r="E134" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H134" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F134" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D135" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E135" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H135" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F135" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D136" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E136" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H136" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F136" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D137" s="5" t="s">
         <v>94</v>
       </c>
       <c r="E137" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H137" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F137" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D138" s="5" t="s">
         <v>95</v>
       </c>
       <c r="E138" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H138" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F138" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D139" s="5" t="s">
         <v>99</v>
       </c>
       <c r="E139" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H139" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F139" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D140" s="5" t="s">
         <v>98</v>
       </c>
       <c r="E140" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H140" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D141" s="5" t="s">
         <v>96</v>
       </c>
       <c r="E141" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H141" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D142" s="5" t="s">
         <v>97</v>
       </c>
       <c r="E142" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H142" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    </row>
+    <row r="143" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="D143" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E143" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H143" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C144" s="15" t="s">
         <v>6</v>
       </c>
@@ -4262,6 +4187,9 @@
       </c>
       <c r="E158" s="5" t="s">
         <v>15</v>
+      </c>
+      <c r="F158" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4273,6 +4201,9 @@
       <c r="E159" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="F159" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B160" s="6"/>
@@ -4282,6 +4213,9 @@
       </c>
       <c r="E160" s="5" t="s">
         <v>15</v>
+      </c>
+      <c r="F160" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="161" spans="1:6" ht="150" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
el script para que cambie dinamicamente el precio total.. lo hice de la naaaaaaaaaaaaada.. de la naaaaaaaaaaaada :'( jajaja xD
</commit_message>
<xml_diff>
--- a/Consigna/correcciones20162C.xlsx
+++ b/Consigna/correcciones20162C.xlsx
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="160">
   <si>
     <t xml:space="preserve">Página de inicio​ (​/default.aspx​)  </t>
   </si>
@@ -651,9 +651,6 @@
     <t>hacer esto</t>
   </si>
   <si>
-    <t>terminar estooo</t>
-  </si>
-  <si>
     <t>no lo redenderiza como checkbox, sino como listbox..</t>
   </si>
   <si>
@@ -661,6 +658,30 @@
   </si>
   <si>
     <t>???????</t>
+  </si>
+  <si>
+    <t>falta lo de la api de google</t>
+  </si>
+  <si>
+    <t xml:space="preserve">falta cargar la imagen.. </t>
+  </si>
+  <si>
+    <t>terminar</t>
+  </si>
+  <si>
+    <t>estos</t>
+  </si>
+  <si>
+    <t>que</t>
+  </si>
+  <si>
+    <t>son</t>
+  </si>
+  <si>
+    <t>una</t>
+  </si>
+  <si>
+    <t>boludes</t>
   </si>
 </sst>
 </file>
@@ -809,6 +830,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -816,15 +846,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2495,10 +2516,10 @@
   <dimension ref="A1:O181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B127" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B148" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M122" sqref="M122"/>
+      <selection pane="bottomRight" activeCell="K146" sqref="K146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2545,14 +2566,14 @@
       </c>
       <c r="K1">
         <f>COUNTIF(F:F, "B")</f>
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>146</v>
       </c>
       <c r="M1" s="14">
         <f>K1/I1</f>
-        <v>0.78417266187050361</v>
+        <v>0.81294964028776984</v>
       </c>
       <c r="N1" s="13" t="s">
         <v>137</v>
@@ -2566,15 +2587,15 @@
       <c r="A2" s="11">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20"/>
     </row>
     <row r="3" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -2620,25 +2641,25 @@
       <c r="A6" s="11">
         <v>1</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="17"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="20"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="17"/>
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2702,12 +2723,12 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="20"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D14" s="5" t="s">
@@ -2722,12 +2743,12 @@
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8"/>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="20"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="17"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D16" s="5" t="s">
@@ -2787,13 +2808,13 @@
       <c r="A22" s="11">
         <v>2</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="17"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D23" s="5" t="s">
@@ -2874,10 +2895,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="20"/>
+      <c r="D30" s="17"/>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D31" s="9" t="s">
@@ -2905,13 +2926,13 @@
       <c r="A33" s="11">
         <v>3</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="17"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="20"/>
     </row>
     <row r="34" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D34" s="4" t="s">
@@ -2974,12 +2995,12 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39" s="8"/>
-      <c r="C39" s="18" t="s">
+      <c r="C39" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="20"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="17"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" s="8"/>
@@ -3080,12 +3101,12 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B48" s="8"/>
-      <c r="C48" s="18" t="s">
+      <c r="C48" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="20"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="17"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
@@ -3128,15 +3149,15 @@
       <c r="A52" s="11">
         <v>4</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B52" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16" t="s">
+      <c r="C52" s="19"/>
+      <c r="D52" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E52" s="16"/>
-      <c r="F52" s="17"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="20"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D53" s="4" t="s">
@@ -3187,12 +3208,12 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C57" s="18" t="s">
+      <c r="C57" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="20"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="17"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D58" s="5" t="s">
@@ -3236,12 +3257,12 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C62" s="18" t="s">
+      <c r="C62" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D62" s="19"/>
-      <c r="E62" s="19"/>
-      <c r="F62" s="20"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="17"/>
     </row>
     <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D63" s="5" t="s">
@@ -3258,15 +3279,15 @@
       <c r="A64" s="11">
         <v>5</v>
       </c>
-      <c r="B64" s="15" t="s">
+      <c r="B64" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C64" s="16" t="s">
+      <c r="C64" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="17"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="20"/>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D65" s="4" t="s">
@@ -3314,12 +3335,12 @@
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C69" s="18" t="s">
+      <c r="C69" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D69" s="19"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="20"/>
+      <c r="D69" s="16"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="17"/>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D70" s="5" t="s">
@@ -3538,7 +3559,7 @@
         <v>15</v>
       </c>
       <c r="H89" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -3586,12 +3607,12 @@
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C94" s="18" t="s">
+      <c r="C94" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D94" s="19"/>
-      <c r="E94" s="19"/>
-      <c r="F94" s="20"/>
+      <c r="D94" s="16"/>
+      <c r="E94" s="16"/>
+      <c r="F94" s="17"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D95" s="5" t="s">
@@ -3608,15 +3629,15 @@
       <c r="A96" s="11">
         <v>6</v>
       </c>
-      <c r="B96" s="15" t="s">
+      <c r="B96" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C96" s="16" t="s">
+      <c r="C96" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="D96" s="16"/>
-      <c r="E96" s="16"/>
-      <c r="F96" s="17"/>
+      <c r="D96" s="19"/>
+      <c r="E96" s="19"/>
+      <c r="F96" s="20"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D97" s="4" t="s">
@@ -3667,12 +3688,12 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C101" s="18" t="s">
+      <c r="C101" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D101" s="19"/>
-      <c r="E101" s="19"/>
-      <c r="F101" s="20"/>
+      <c r="D101" s="16"/>
+      <c r="E101" s="16"/>
+      <c r="F101" s="17"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D102" s="5" t="s">
@@ -3743,12 +3764,12 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C108" s="18" t="s">
+      <c r="C108" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D108" s="19"/>
-      <c r="E108" s="19"/>
-      <c r="F108" s="20"/>
+      <c r="D108" s="16"/>
+      <c r="E108" s="16"/>
+      <c r="F108" s="17"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D109" s="5" t="s">
@@ -3765,15 +3786,15 @@
       <c r="A110" s="11">
         <v>7</v>
       </c>
-      <c r="B110" s="15" t="s">
+      <c r="B110" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C110" s="16" t="s">
+      <c r="C110" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="D110" s="16"/>
-      <c r="E110" s="16"/>
-      <c r="F110" s="17"/>
+      <c r="D110" s="19"/>
+      <c r="E110" s="19"/>
+      <c r="F110" s="20"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D111" s="4" t="s">
@@ -3834,16 +3855,16 @@
         <v>139</v>
       </c>
       <c r="H115" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C116" s="18" t="s">
+      <c r="C116" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D116" s="19"/>
-      <c r="E116" s="19"/>
-      <c r="F116" s="20"/>
+      <c r="D116" s="16"/>
+      <c r="E116" s="16"/>
+      <c r="F116" s="17"/>
     </row>
     <row r="117" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C117" s="7"/>
@@ -3881,12 +3902,12 @@
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C120" s="18" t="s">
+      <c r="C120" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D120" s="19"/>
-      <c r="E120" s="19"/>
-      <c r="F120" s="20"/>
+      <c r="D120" s="16"/>
+      <c r="E120" s="16"/>
+      <c r="F120" s="17"/>
     </row>
     <row r="121" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D121" s="5" t="s">
@@ -3896,22 +3917,22 @@
         <v>15</v>
       </c>
       <c r="H121" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="11">
         <v>8</v>
       </c>
-      <c r="B122" s="15" t="s">
+      <c r="B122" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="C122" s="16" t="s">
+      <c r="C122" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D122" s="16"/>
-      <c r="E122" s="16"/>
-      <c r="F122" s="17"/>
+      <c r="D122" s="19"/>
+      <c r="E122" s="19"/>
+      <c r="F122" s="20"/>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D123" s="4" t="s">
@@ -3957,6 +3978,9 @@
       <c r="E126" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="H126" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D127" s="5" t="s">
@@ -3970,14 +3994,14 @@
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C128" s="18" t="s">
+      <c r="C128" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D128" s="19"/>
-      <c r="E128" s="19"/>
-      <c r="F128" s="20"/>
-    </row>
-    <row r="129" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D128" s="16"/>
+      <c r="E128" s="16"/>
+      <c r="F128" s="17"/>
+    </row>
+    <row r="129" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="C129" s="7"/>
       <c r="D129" s="5" t="s">
         <v>135</v>
@@ -3989,21 +4013,21 @@
         <v>139</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="11">
         <v>8.1</v>
       </c>
-      <c r="B130" s="15" t="s">
+      <c r="B130" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="C130" s="16" t="s">
+      <c r="C130" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="D130" s="16"/>
-      <c r="E130" s="16"/>
-      <c r="F130" s="17"/>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D130" s="19"/>
+      <c r="E130" s="19"/>
+      <c r="F130" s="20"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D131" s="4" t="s">
         <v>1</v>
       </c>
@@ -4014,7 +4038,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="6"/>
       <c r="C132" s="6"/>
       <c r="D132" s="4" t="s">
@@ -4027,7 +4051,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B133" s="6"/>
       <c r="C133" s="6"/>
       <c r="D133" s="4" t="s">
@@ -4040,7 +4064,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="D134" s="5" t="s">
         <v>92</v>
       </c>
@@ -4051,7 +4075,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D135" s="5" t="s">
         <v>49</v>
       </c>
@@ -4062,7 +4086,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D136" s="5" t="s">
         <v>50</v>
       </c>
@@ -4073,7 +4097,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D137" s="5" t="s">
         <v>94</v>
       </c>
@@ -4084,7 +4108,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D138" s="5" t="s">
         <v>95</v>
       </c>
@@ -4095,7 +4119,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D139" s="5" t="s">
         <v>99</v>
       </c>
@@ -4106,45 +4130,60 @@
         <v>139</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D140" s="5" t="s">
         <v>98</v>
       </c>
       <c r="E140" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F140" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="H140" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D141" s="5" t="s">
         <v>96</v>
       </c>
       <c r="E141" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F141" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D142" s="5" t="s">
         <v>97</v>
       </c>
       <c r="E142" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="F142" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="D143" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E143" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C144" s="18" t="s">
+      <c r="F143" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C144" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D144" s="19"/>
-      <c r="E144" s="19"/>
-      <c r="F144" s="20"/>
+      <c r="D144" s="16"/>
+      <c r="E144" s="16"/>
+      <c r="F144" s="17"/>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D145" s="5" t="s">
@@ -4154,7 +4193,7 @@
         <v>15</v>
       </c>
       <c r="H145" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="146" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4164,6 +4203,9 @@
       <c r="E146" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="H146" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D147" s="5" t="s">
@@ -4172,6 +4214,9 @@
       <c r="E147" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="H147" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D148" s="5" t="s">
@@ -4180,6 +4225,9 @@
       <c r="E148" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="H148" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D149" s="5" t="s">
@@ -4188,6 +4236,9 @@
       <c r="E149" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="H149" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D150" s="5" t="s">
@@ -4196,6 +4247,9 @@
       <c r="E150" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="H150" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D151" s="5" t="s">
@@ -4222,12 +4276,12 @@
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C154" s="18" t="s">
+      <c r="C154" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D154" s="19"/>
-      <c r="E154" s="19"/>
-      <c r="F154" s="20"/>
+      <c r="D154" s="16"/>
+      <c r="E154" s="16"/>
+      <c r="F154" s="17"/>
     </row>
     <row r="155" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D155" s="5" t="s">
@@ -4249,15 +4303,15 @@
       <c r="A157" s="11">
         <v>9</v>
       </c>
-      <c r="B157" s="15" t="s">
+      <c r="B157" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C157" s="16" t="s">
+      <c r="C157" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="D157" s="16"/>
-      <c r="E157" s="16"/>
-      <c r="F157" s="17"/>
+      <c r="D157" s="19"/>
+      <c r="E157" s="19"/>
+      <c r="F157" s="20"/>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D158" s="4" t="s">
@@ -4348,15 +4402,15 @@
       <c r="A167" s="11">
         <v>10</v>
       </c>
-      <c r="B167" s="15" t="s">
+      <c r="B167" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C167" s="16" t="s">
+      <c r="C167" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="D167" s="16"/>
-      <c r="E167" s="16"/>
-      <c r="F167" s="17"/>
+      <c r="D167" s="19"/>
+      <c r="E167" s="19"/>
+      <c r="F167" s="20"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D168" s="4" t="s">
@@ -4430,15 +4484,15 @@
       <c r="A176" s="11">
         <v>11</v>
       </c>
-      <c r="B176" s="15" t="s">
+      <c r="B176" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="C176" s="16" t="s">
+      <c r="C176" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="D176" s="16"/>
-      <c r="E176" s="16"/>
-      <c r="F176" s="17"/>
+      <c r="D176" s="19"/>
+      <c r="E176" s="19"/>
+      <c r="F176" s="20"/>
     </row>
     <row r="177" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D177" s="5" t="s">
@@ -4497,20 +4551,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C62:F62"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C154:F154"/>
-    <mergeCell ref="B167:F167"/>
-    <mergeCell ref="B176:F176"/>
-    <mergeCell ref="B157:F157"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C69:F69"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="C108:F108"/>
-    <mergeCell ref="C116:F116"/>
-    <mergeCell ref="C120:F120"/>
-    <mergeCell ref="C128:F128"/>
-    <mergeCell ref="C144:F144"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B22:F22"/>
@@ -4527,6 +4567,20 @@
     <mergeCell ref="C39:F39"/>
     <mergeCell ref="C48:F48"/>
     <mergeCell ref="C57:F57"/>
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C154:F154"/>
+    <mergeCell ref="B167:F167"/>
+    <mergeCell ref="B176:F176"/>
+    <mergeCell ref="B157:F157"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C69:F69"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="C108:F108"/>
+    <mergeCell ref="C116:F116"/>
+    <mergeCell ref="C120:F120"/>
+    <mergeCell ref="C128:F128"/>
+    <mergeCell ref="C144:F144"/>
   </mergeCells>
   <conditionalFormatting sqref="E16:E21 E149:E153 E1 E11:E12 E37:E38 E56 E100 E161:E166 E171:E175 E14 E23:E32 E40:E47 E63 E49:E51 E58:E61 E68 E81:E93 E70:E78 E102:E107 E117:E119 E121 E129 E95 E109 E114:E115 E134:E143 E155:E156 E3:E5 E126:E127 E177:E1048576">
     <cfRule type="cellIs" dxfId="134" priority="140" operator="equal">

</xml_diff>

<commit_message>
abre modal de puntuacion y manda por hidden field el valor del seleccionado
</commit_message>
<xml_diff>
--- a/Consigna/correcciones20162C.xlsx
+++ b/Consigna/correcciones20162C.xlsx
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="155">
   <si>
     <t xml:space="preserve">Página de inicio​ (​/default.aspx​)  </t>
   </si>
@@ -664,6 +664,9 @@
   </si>
   <si>
     <t xml:space="preserve">falta cargar la imagen.. </t>
+  </si>
+  <si>
+    <t>hacer.. Una boludes</t>
   </si>
 </sst>
 </file>
@@ -812,6 +815,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -819,15 +831,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2498,10 +2501,10 @@
   <dimension ref="A1:O181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B165" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B160" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G169" sqref="G169"/>
+      <selection pane="bottomRight" activeCell="J161" sqref="J161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2548,14 +2551,14 @@
       </c>
       <c r="K1">
         <f>COUNTIF(F:F, "B")</f>
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>146</v>
       </c>
       <c r="M1" s="14">
         <f>K1/I1</f>
-        <v>0.8848920863309353</v>
+        <v>0.93525179856115104</v>
       </c>
       <c r="N1" s="13" t="s">
         <v>137</v>
@@ -2569,15 +2572,15 @@
       <c r="A2" s="11">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20"/>
     </row>
     <row r="3" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -2623,25 +2626,25 @@
       <c r="A6" s="11">
         <v>1</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="17"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="20"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="17"/>
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2705,12 +2708,12 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="20"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D14" s="5" t="s">
@@ -2725,12 +2728,12 @@
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8"/>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="20"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="17"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D16" s="5" t="s">
@@ -2790,13 +2793,13 @@
       <c r="A22" s="11">
         <v>2</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="17"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D23" s="5" t="s">
@@ -2877,10 +2880,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="20"/>
+      <c r="D30" s="17"/>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D31" s="9" t="s">
@@ -2908,13 +2911,13 @@
       <c r="A33" s="11">
         <v>3</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="17"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="20"/>
     </row>
     <row r="34" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D34" s="4" t="s">
@@ -2977,12 +2980,12 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39" s="8"/>
-      <c r="C39" s="18" t="s">
+      <c r="C39" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="20"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="17"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" s="8"/>
@@ -3083,12 +3086,12 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B48" s="8"/>
-      <c r="C48" s="18" t="s">
+      <c r="C48" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="20"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="17"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
@@ -3131,15 +3134,15 @@
       <c r="A52" s="11">
         <v>4</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B52" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16" t="s">
+      <c r="C52" s="19"/>
+      <c r="D52" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E52" s="16"/>
-      <c r="F52" s="17"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="20"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D53" s="4" t="s">
@@ -3190,12 +3193,12 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C57" s="18" t="s">
+      <c r="C57" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="20"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="17"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D58" s="5" t="s">
@@ -3239,12 +3242,12 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C62" s="18" t="s">
+      <c r="C62" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D62" s="19"/>
-      <c r="E62" s="19"/>
-      <c r="F62" s="20"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="17"/>
     </row>
     <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D63" s="5" t="s">
@@ -3261,15 +3264,15 @@
       <c r="A64" s="11">
         <v>5</v>
       </c>
-      <c r="B64" s="15" t="s">
+      <c r="B64" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C64" s="16" t="s">
+      <c r="C64" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="17"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="20"/>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D65" s="4" t="s">
@@ -3317,12 +3320,12 @@
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C69" s="18" t="s">
+      <c r="C69" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D69" s="19"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="20"/>
+      <c r="D69" s="16"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="17"/>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D70" s="5" t="s">
@@ -3589,12 +3592,12 @@
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C94" s="18" t="s">
+      <c r="C94" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D94" s="19"/>
-      <c r="E94" s="19"/>
-      <c r="F94" s="20"/>
+      <c r="D94" s="16"/>
+      <c r="E94" s="16"/>
+      <c r="F94" s="17"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D95" s="5" t="s">
@@ -3611,15 +3614,15 @@
       <c r="A96" s="11">
         <v>6</v>
       </c>
-      <c r="B96" s="15" t="s">
+      <c r="B96" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C96" s="16" t="s">
+      <c r="C96" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="D96" s="16"/>
-      <c r="E96" s="16"/>
-      <c r="F96" s="17"/>
+      <c r="D96" s="19"/>
+      <c r="E96" s="19"/>
+      <c r="F96" s="20"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D97" s="4" t="s">
@@ -3670,12 +3673,12 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C101" s="18" t="s">
+      <c r="C101" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D101" s="19"/>
-      <c r="E101" s="19"/>
-      <c r="F101" s="20"/>
+      <c r="D101" s="16"/>
+      <c r="E101" s="16"/>
+      <c r="F101" s="17"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D102" s="5" t="s">
@@ -3746,12 +3749,12 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C108" s="18" t="s">
+      <c r="C108" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D108" s="19"/>
-      <c r="E108" s="19"/>
-      <c r="F108" s="20"/>
+      <c r="D108" s="16"/>
+      <c r="E108" s="16"/>
+      <c r="F108" s="17"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D109" s="5" t="s">
@@ -3768,15 +3771,15 @@
       <c r="A110" s="11">
         <v>7</v>
       </c>
-      <c r="B110" s="15" t="s">
+      <c r="B110" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C110" s="16" t="s">
+      <c r="C110" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="D110" s="16"/>
-      <c r="E110" s="16"/>
-      <c r="F110" s="17"/>
+      <c r="D110" s="19"/>
+      <c r="E110" s="19"/>
+      <c r="F110" s="20"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D111" s="4" t="s">
@@ -3841,12 +3844,12 @@
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C116" s="18" t="s">
+      <c r="C116" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D116" s="19"/>
-      <c r="E116" s="19"/>
-      <c r="F116" s="20"/>
+      <c r="D116" s="16"/>
+      <c r="E116" s="16"/>
+      <c r="F116" s="17"/>
     </row>
     <row r="117" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C117" s="7"/>
@@ -3884,12 +3887,12 @@
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C120" s="18" t="s">
+      <c r="C120" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D120" s="19"/>
-      <c r="E120" s="19"/>
-      <c r="F120" s="20"/>
+      <c r="D120" s="16"/>
+      <c r="E120" s="16"/>
+      <c r="F120" s="17"/>
     </row>
     <row r="121" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D121" s="5" t="s">
@@ -3906,15 +3909,15 @@
       <c r="A122" s="11">
         <v>8</v>
       </c>
-      <c r="B122" s="15" t="s">
+      <c r="B122" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="C122" s="16" t="s">
+      <c r="C122" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D122" s="16"/>
-      <c r="E122" s="16"/>
-      <c r="F122" s="17"/>
+      <c r="D122" s="19"/>
+      <c r="E122" s="19"/>
+      <c r="F122" s="20"/>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D123" s="4" t="s">
@@ -3976,12 +3979,12 @@
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C128" s="18" t="s">
+      <c r="C128" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D128" s="19"/>
-      <c r="E128" s="19"/>
-      <c r="F128" s="20"/>
+      <c r="D128" s="16"/>
+      <c r="E128" s="16"/>
+      <c r="F128" s="17"/>
     </row>
     <row r="129" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="C129" s="7"/>
@@ -3999,15 +4002,15 @@
       <c r="A130" s="11">
         <v>8.1</v>
       </c>
-      <c r="B130" s="15" t="s">
+      <c r="B130" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="C130" s="16" t="s">
+      <c r="C130" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="D130" s="16"/>
-      <c r="E130" s="16"/>
-      <c r="F130" s="17"/>
+      <c r="D130" s="19"/>
+      <c r="E130" s="19"/>
+      <c r="F130" s="20"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D131" s="4" t="s">
@@ -4160,12 +4163,12 @@
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C144" s="18" t="s">
+      <c r="C144" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D144" s="19"/>
-      <c r="E144" s="19"/>
-      <c r="F144" s="20"/>
+      <c r="D144" s="16"/>
+      <c r="E144" s="16"/>
+      <c r="F144" s="17"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D145" s="5" t="s">
@@ -4264,12 +4267,12 @@
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C154" s="18" t="s">
+      <c r="C154" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D154" s="19"/>
-      <c r="E154" s="19"/>
-      <c r="F154" s="20"/>
+      <c r="D154" s="16"/>
+      <c r="E154" s="16"/>
+      <c r="F154" s="17"/>
     </row>
     <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D155" s="5" t="s">
@@ -4297,15 +4300,15 @@
       <c r="A157" s="11">
         <v>9</v>
       </c>
-      <c r="B157" s="15" t="s">
+      <c r="B157" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C157" s="16" t="s">
+      <c r="C157" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="D157" s="16"/>
-      <c r="E157" s="16"/>
-      <c r="F157" s="17"/>
+      <c r="D157" s="19"/>
+      <c r="E157" s="19"/>
+      <c r="F157" s="20"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D158" s="4" t="s">
@@ -4344,15 +4347,18 @@
         <v>139</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="D161" s="5" t="s">
         <v>108</v>
       </c>
       <c r="E161" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F161" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D162" s="5" t="s">
         <v>112</v>
       </c>
@@ -4360,7 +4366,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D163" s="5" t="s">
         <v>113</v>
       </c>
@@ -4368,23 +4374,29 @@
         <v>131</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D164" s="5" t="s">
         <v>109</v>
       </c>
       <c r="E164" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H164" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D165" s="5" t="s">
         <v>111</v>
       </c>
       <c r="E165" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F165" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D166" s="5" t="s">
         <v>110</v>
       </c>
@@ -4392,29 +4404,32 @@
         <v>131</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="11">
         <v>10</v>
       </c>
-      <c r="B167" s="15" t="s">
+      <c r="B167" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C167" s="16" t="s">
+      <c r="C167" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="D167" s="16"/>
-      <c r="E167" s="16"/>
-      <c r="F167" s="17"/>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D167" s="19"/>
+      <c r="E167" s="19"/>
+      <c r="F167" s="20"/>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D168" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E168" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F168" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B169" s="6"/>
       <c r="C169" s="6"/>
       <c r="D169" s="4" t="s">
@@ -4423,8 +4438,11 @@
       <c r="E169" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F169" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B170" s="6"/>
       <c r="C170" s="6"/>
       <c r="D170" s="4" t="s">
@@ -4433,8 +4451,11 @@
       <c r="E170" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F170" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D171" s="5" t="s">
         <v>115</v>
       </c>
@@ -4442,7 +4463,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D172" s="5" t="s">
         <v>116</v>
       </c>
@@ -4450,23 +4471,29 @@
         <v>131</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D173" s="5" t="s">
         <v>117</v>
       </c>
       <c r="E173" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F173" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D174" s="5" t="s">
         <v>118</v>
       </c>
       <c r="E174" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F174" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D175" s="5" t="s">
         <v>119</v>
       </c>
@@ -4474,19 +4501,19 @@
         <v>131</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="11">
         <v>11</v>
       </c>
-      <c r="B176" s="15" t="s">
+      <c r="B176" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="C176" s="16" t="s">
+      <c r="C176" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="D176" s="16"/>
-      <c r="E176" s="16"/>
-      <c r="F176" s="17"/>
+      <c r="D176" s="19"/>
+      <c r="E176" s="19"/>
+      <c r="F176" s="20"/>
     </row>
     <row r="177" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D177" s="5" t="s">
@@ -4545,20 +4572,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C62:F62"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C154:F154"/>
-    <mergeCell ref="B167:F167"/>
-    <mergeCell ref="B176:F176"/>
-    <mergeCell ref="B157:F157"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C69:F69"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="C108:F108"/>
-    <mergeCell ref="C116:F116"/>
-    <mergeCell ref="C120:F120"/>
-    <mergeCell ref="C128:F128"/>
-    <mergeCell ref="C144:F144"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B22:F22"/>
@@ -4575,6 +4588,20 @@
     <mergeCell ref="C39:F39"/>
     <mergeCell ref="C48:F48"/>
     <mergeCell ref="C57:F57"/>
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C154:F154"/>
+    <mergeCell ref="B167:F167"/>
+    <mergeCell ref="B176:F176"/>
+    <mergeCell ref="B157:F157"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C69:F69"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="C108:F108"/>
+    <mergeCell ref="C116:F116"/>
+    <mergeCell ref="C120:F120"/>
+    <mergeCell ref="C128:F128"/>
+    <mergeCell ref="C144:F144"/>
   </mergeCells>
   <conditionalFormatting sqref="E16:E21 E149:E153 E1 E11:E12 E37:E38 E56 E100 E161:E166 E171:E175 E14 E23:E32 E40:E47 E63 E49:E51 E58:E61 E68 E81:E93 E70:E78 E102:E107 E117:E119 E121 E129 E95 E109 E114:E115 E134:E143 E155:E156 E3:E5 E126:E127 E177:E1048576">
     <cfRule type="cellIs" dxfId="134" priority="140" operator="equal">

</xml_diff>

<commit_message>
Mapa y Foto en la Grilla en default y en clienteReservar minor bug fixed(? xD
</commit_message>
<xml_diff>
--- a/Consigna/correcciones20162C.xlsx
+++ b/Consigna/correcciones20162C.xlsx
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="151">
   <si>
     <t xml:space="preserve">Página de inicio​ (​/default.aspx​)  </t>
   </si>
@@ -654,13 +654,7 @@
     <t>no se puede hacer sin base de datos.. Pero se simula</t>
   </si>
   <si>
-    <t>???????</t>
-  </si>
-  <si>
     <t xml:space="preserve">falta cargar la imagen.. </t>
-  </si>
-  <si>
-    <t>falta lo de la api de google que parece que es paga..</t>
   </si>
 </sst>
 </file>
@@ -809,6 +803,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -816,15 +819,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2495,10 +2489,10 @@
   <dimension ref="A1:O181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B126" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B127" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H121" sqref="H121"/>
+      <selection pane="bottomRight" activeCell="K124" sqref="K124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2545,14 +2539,14 @@
       </c>
       <c r="K1">
         <f>COUNTIF(F:F, "B")</f>
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>146</v>
       </c>
       <c r="M1" s="14">
         <f>K1/I1</f>
-        <v>0.95683453237410077</v>
+        <v>0.97122302158273377</v>
       </c>
       <c r="N1" s="13" t="s">
         <v>137</v>
@@ -2566,15 +2560,15 @@
       <c r="A2" s="11">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="3" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -2620,25 +2614,25 @@
       <c r="A6" s="11">
         <v>1</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="17"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="20"/>
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2702,12 +2696,12 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="20"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D14" s="5" t="s">
@@ -2722,12 +2716,12 @@
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8"/>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="20"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D16" s="5" t="s">
@@ -2787,13 +2781,13 @@
       <c r="A22" s="11">
         <v>2</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="20"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="17"/>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D23" s="5" t="s">
@@ -2874,10 +2868,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="17"/>
+      <c r="D30" s="20"/>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D31" s="9" t="s">
@@ -2905,13 +2899,13 @@
       <c r="A33" s="11">
         <v>3</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="20"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="17"/>
     </row>
     <row r="34" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D34" s="4" t="s">
@@ -2974,12 +2968,12 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39" s="8"/>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="17"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="20"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" s="8"/>
@@ -3080,12 +3074,12 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B48" s="8"/>
-      <c r="C48" s="15" t="s">
+      <c r="C48" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D48" s="16"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="17"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="20"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
@@ -3128,15 +3122,15 @@
       <c r="A52" s="11">
         <v>4</v>
       </c>
-      <c r="B52" s="18" t="s">
+      <c r="B52" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19" t="s">
+      <c r="C52" s="16"/>
+      <c r="D52" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E52" s="19"/>
-      <c r="F52" s="20"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="17"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D53" s="4" t="s">
@@ -3187,12 +3181,12 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C57" s="15" t="s">
+      <c r="C57" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D57" s="16"/>
-      <c r="E57" s="16"/>
-      <c r="F57" s="17"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="20"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D58" s="5" t="s">
@@ -3236,12 +3230,12 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C62" s="15" t="s">
+      <c r="C62" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="17"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="20"/>
     </row>
     <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D63" s="5" t="s">
@@ -3258,15 +3252,15 @@
       <c r="A64" s="11">
         <v>5</v>
       </c>
-      <c r="B64" s="18" t="s">
+      <c r="B64" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C64" s="19" t="s">
+      <c r="C64" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D64" s="19"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="20"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="17"/>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D65" s="4" t="s">
@@ -3317,12 +3311,12 @@
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C69" s="15" t="s">
+      <c r="C69" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D69" s="16"/>
-      <c r="E69" s="16"/>
-      <c r="F69" s="17"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="20"/>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D70" s="5" t="s">
@@ -3589,12 +3583,12 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C94" s="15" t="s">
+      <c r="C94" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D94" s="16"/>
-      <c r="E94" s="16"/>
-      <c r="F94" s="17"/>
+      <c r="D94" s="19"/>
+      <c r="E94" s="19"/>
+      <c r="F94" s="20"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D95" s="5" t="s">
@@ -3611,15 +3605,15 @@
       <c r="A96" s="11">
         <v>6</v>
       </c>
-      <c r="B96" s="18" t="s">
+      <c r="B96" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C96" s="19" t="s">
+      <c r="C96" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="D96" s="19"/>
-      <c r="E96" s="19"/>
-      <c r="F96" s="20"/>
+      <c r="D96" s="16"/>
+      <c r="E96" s="16"/>
+      <c r="F96" s="17"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D97" s="4" t="s">
@@ -3670,12 +3664,12 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C101" s="15" t="s">
+      <c r="C101" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D101" s="16"/>
-      <c r="E101" s="16"/>
-      <c r="F101" s="17"/>
+      <c r="D101" s="19"/>
+      <c r="E101" s="19"/>
+      <c r="F101" s="20"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D102" s="5" t="s">
@@ -3746,12 +3740,12 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C108" s="15" t="s">
+      <c r="C108" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D108" s="16"/>
-      <c r="E108" s="16"/>
-      <c r="F108" s="17"/>
+      <c r="D108" s="19"/>
+      <c r="E108" s="19"/>
+      <c r="F108" s="20"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D109" s="5" t="s">
@@ -3768,15 +3762,15 @@
       <c r="A110" s="11">
         <v>7</v>
       </c>
-      <c r="B110" s="18" t="s">
+      <c r="B110" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C110" s="19" t="s">
+      <c r="C110" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="D110" s="19"/>
-      <c r="E110" s="19"/>
-      <c r="F110" s="20"/>
+      <c r="D110" s="16"/>
+      <c r="E110" s="16"/>
+      <c r="F110" s="17"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D111" s="4" t="s">
@@ -3841,12 +3835,12 @@
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C116" s="15" t="s">
+      <c r="C116" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D116" s="16"/>
-      <c r="E116" s="16"/>
-      <c r="F116" s="17"/>
+      <c r="D116" s="19"/>
+      <c r="E116" s="19"/>
+      <c r="F116" s="20"/>
     </row>
     <row r="117" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C117" s="7"/>
@@ -3884,12 +3878,12 @@
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C120" s="15" t="s">
+      <c r="C120" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D120" s="16"/>
-      <c r="E120" s="16"/>
-      <c r="F120" s="17"/>
+      <c r="D120" s="19"/>
+      <c r="E120" s="19"/>
+      <c r="F120" s="20"/>
     </row>
     <row r="121" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D121" s="5" t="s">
@@ -3898,23 +3892,23 @@
       <c r="E121" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H121" t="s">
-        <v>150</v>
+      <c r="F121" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="11">
         <v>8</v>
       </c>
-      <c r="B122" s="18" t="s">
+      <c r="B122" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="C122" s="19" t="s">
+      <c r="C122" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="D122" s="19"/>
-      <c r="E122" s="19"/>
-      <c r="F122" s="20"/>
+      <c r="D122" s="16"/>
+      <c r="E122" s="16"/>
+      <c r="F122" s="17"/>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D123" s="4" t="s">
@@ -3960,8 +3954,8 @@
       <c r="E126" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H126" t="s">
-        <v>152</v>
+      <c r="F126" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -3976,12 +3970,12 @@
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C128" s="15" t="s">
+      <c r="C128" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D128" s="16"/>
-      <c r="E128" s="16"/>
-      <c r="F128" s="17"/>
+      <c r="D128" s="19"/>
+      <c r="E128" s="19"/>
+      <c r="F128" s="20"/>
     </row>
     <row r="129" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="C129" s="7"/>
@@ -3999,15 +3993,15 @@
       <c r="A130" s="11">
         <v>8.1</v>
       </c>
-      <c r="B130" s="18" t="s">
+      <c r="B130" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="C130" s="19" t="s">
+      <c r="C130" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="D130" s="19"/>
-      <c r="E130" s="19"/>
-      <c r="F130" s="20"/>
+      <c r="D130" s="16"/>
+      <c r="E130" s="16"/>
+      <c r="F130" s="17"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D131" s="4" t="s">
@@ -4123,7 +4117,7 @@
         <v>139</v>
       </c>
       <c r="H140" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
@@ -4160,12 +4154,12 @@
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C144" s="15" t="s">
+      <c r="C144" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D144" s="16"/>
-      <c r="E144" s="16"/>
-      <c r="F144" s="17"/>
+      <c r="D144" s="19"/>
+      <c r="E144" s="19"/>
+      <c r="F144" s="20"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D145" s="5" t="s">
@@ -4264,12 +4258,12 @@
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C154" s="15" t="s">
+      <c r="C154" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D154" s="16"/>
-      <c r="E154" s="16"/>
-      <c r="F154" s="17"/>
+      <c r="D154" s="19"/>
+      <c r="E154" s="19"/>
+      <c r="F154" s="20"/>
     </row>
     <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D155" s="5" t="s">
@@ -4297,15 +4291,15 @@
       <c r="A157" s="11">
         <v>9</v>
       </c>
-      <c r="B157" s="18" t="s">
+      <c r="B157" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="C157" s="19" t="s">
+      <c r="C157" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="D157" s="19"/>
-      <c r="E157" s="19"/>
-      <c r="F157" s="20"/>
+      <c r="D157" s="16"/>
+      <c r="E157" s="16"/>
+      <c r="F157" s="17"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D158" s="4" t="s">
@@ -4405,15 +4399,15 @@
       <c r="A167" s="11">
         <v>10</v>
       </c>
-      <c r="B167" s="18" t="s">
+      <c r="B167" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C167" s="19" t="s">
+      <c r="C167" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="D167" s="19"/>
-      <c r="E167" s="19"/>
-      <c r="F167" s="20"/>
+      <c r="D167" s="16"/>
+      <c r="E167" s="16"/>
+      <c r="F167" s="17"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D168" s="4" t="s">
@@ -4502,15 +4496,15 @@
       <c r="A176" s="11">
         <v>11</v>
       </c>
-      <c r="B176" s="18" t="s">
+      <c r="B176" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="C176" s="19" t="s">
+      <c r="C176" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="D176" s="19"/>
-      <c r="E176" s="19"/>
-      <c r="F176" s="20"/>
+      <c r="D176" s="16"/>
+      <c r="E176" s="16"/>
+      <c r="F176" s="17"/>
     </row>
     <row r="177" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D177" s="5" t="s">
@@ -4569,6 +4563,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C154:F154"/>
+    <mergeCell ref="B167:F167"/>
+    <mergeCell ref="B176:F176"/>
+    <mergeCell ref="B157:F157"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C69:F69"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="C108:F108"/>
+    <mergeCell ref="C116:F116"/>
+    <mergeCell ref="C120:F120"/>
+    <mergeCell ref="C128:F128"/>
+    <mergeCell ref="C144:F144"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B22:F22"/>
@@ -4585,20 +4593,6 @@
     <mergeCell ref="C39:F39"/>
     <mergeCell ref="C48:F48"/>
     <mergeCell ref="C57:F57"/>
-    <mergeCell ref="C62:F62"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C154:F154"/>
-    <mergeCell ref="B167:F167"/>
-    <mergeCell ref="B176:F176"/>
-    <mergeCell ref="B157:F157"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C69:F69"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="C108:F108"/>
-    <mergeCell ref="C116:F116"/>
-    <mergeCell ref="C120:F120"/>
-    <mergeCell ref="C128:F128"/>
-    <mergeCell ref="C144:F144"/>
   </mergeCells>
   <conditionalFormatting sqref="E16:E21 E149:E153 E1 E11:E12 E37:E38 E56 E100 E161:E166 E171:E175 E14 E23:E32 E40:E47 E63 E49:E51 E58:E61 E68 E81:E93 E70:E78 E102:E107 E117:E119 E121 E129 E95 E109 E114:E115 E134:E143 E155:E156 E3:E5 E126:E127 E177:E1048576">
     <cfRule type="cellIs" dxfId="134" priority="140" operator="equal">

</xml_diff>

<commit_message>
Listo para la Primera Entrega
</commit_message>
<xml_diff>
--- a/Consigna/correcciones20162C.xlsx
+++ b/Consigna/correcciones20162C.xlsx
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="148">
   <si>
     <t xml:space="preserve">Página de inicio​ (​/default.aspx​)  </t>
   </si>
@@ -646,15 +646,6 @@
   </si>
   <si>
     <t>Enviaron este excel marcando en Correccion, con B lo que pudieron hacer?</t>
-  </si>
-  <si>
-    <t>hacer esto</t>
-  </si>
-  <si>
-    <t>no se puede hacer sin base de datos.. Pero se simula</t>
-  </si>
-  <si>
-    <t xml:space="preserve">falta cargar la imagen.. </t>
   </si>
 </sst>
 </file>
@@ -2489,10 +2480,10 @@
   <dimension ref="A1:O181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B127" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K124" sqref="K124"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2539,14 +2530,14 @@
       </c>
       <c r="K1">
         <f>COUNTIF(F:F, "B")</f>
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>146</v>
       </c>
       <c r="M1" s="14">
         <f>K1/I1</f>
-        <v>0.97122302158273377</v>
+        <v>0.98561151079136688</v>
       </c>
       <c r="N1" s="13" t="s">
         <v>137</v>
@@ -2895,7 +2886,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>3</v>
       </c>
@@ -2907,7 +2898,7 @@
       <c r="E33" s="16"/>
       <c r="F33" s="17"/>
     </row>
-    <row r="34" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D34" s="4" t="s">
         <v>1</v>
       </c>
@@ -2918,7 +2909,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="4" t="s">
@@ -2931,7 +2922,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="4" t="s">
@@ -2944,7 +2935,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D37" s="5" t="s">
         <v>27</v>
       </c>
@@ -2955,7 +2946,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D38" s="5" t="s">
         <v>26</v>
       </c>
@@ -2966,7 +2957,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" s="8"/>
       <c r="C39" s="18" t="s">
         <v>28</v>
@@ -2975,7 +2966,7 @@
       <c r="E39" s="19"/>
       <c r="F39" s="20"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" s="8"/>
       <c r="C40" s="7"/>
       <c r="D40" s="5" t="s">
@@ -2988,7 +2979,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="8"/>
       <c r="C41" s="7"/>
       <c r="D41" s="5" t="s">
@@ -3001,7 +2992,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B42" s="8"/>
       <c r="C42" s="7"/>
       <c r="D42" s="5" t="s">
@@ -3010,8 +3001,11 @@
       <c r="E42" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F42" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" s="8"/>
       <c r="C43" s="7"/>
       <c r="D43" s="5" t="s">
@@ -3024,7 +3018,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B44" s="8"/>
       <c r="C44" s="7"/>
       <c r="D44" s="5" t="s">
@@ -3033,11 +3027,11 @@
       <c r="E44" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H44" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="F44" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D45" s="5" t="s">
         <v>29</v>
       </c>
@@ -3048,7 +3042,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D46" s="5" t="s">
         <v>30</v>
       </c>
@@ -3059,7 +3053,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B47" s="8"/>
       <c r="C47" s="7"/>
       <c r="D47" s="5" t="s">
@@ -3072,7 +3066,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" s="8"/>
       <c r="C48" s="18" t="s">
         <v>6</v>
@@ -3796,7 +3790,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
       <c r="D113" s="4" t="s">
@@ -3809,7 +3803,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="D114" s="5" t="s">
         <v>134</v>
       </c>
@@ -3820,7 +3814,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D115" s="5" t="s">
         <v>88</v>
       </c>
@@ -3830,11 +3824,8 @@
       <c r="F115" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="H115" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C116" s="18" t="s">
         <v>6</v>
       </c>
@@ -3842,7 +3833,7 @@
       <c r="E116" s="19"/>
       <c r="F116" s="20"/>
     </row>
-    <row r="117" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C117" s="7"/>
       <c r="D117" s="5" t="s">
         <v>84</v>
@@ -3854,7 +3845,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C118" s="7"/>
       <c r="D118" s="5" t="s">
         <v>85</v>
@@ -3866,7 +3857,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D119" s="5" t="s">
         <v>83</v>
       </c>
@@ -3877,7 +3868,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C120" s="18" t="s">
         <v>10</v>
       </c>
@@ -3885,7 +3876,7 @@
       <c r="E120" s="19"/>
       <c r="F120" s="20"/>
     </row>
-    <row r="121" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D121" s="5" t="s">
         <v>86</v>
       </c>
@@ -3896,7 +3887,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="11">
         <v>8</v>
       </c>
@@ -3910,7 +3901,7 @@
       <c r="E122" s="16"/>
       <c r="F122" s="17"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D123" s="4" t="s">
         <v>1</v>
       </c>
@@ -3921,7 +3912,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" s="6"/>
       <c r="C124" s="6"/>
       <c r="D124" s="4" t="s">
@@ -3934,7 +3925,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B125" s="6"/>
       <c r="C125" s="6"/>
       <c r="D125" s="4" t="s">
@@ -3947,7 +3938,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="D126" s="5" t="s">
         <v>90</v>
       </c>
@@ -3958,7 +3949,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D127" s="5" t="s">
         <v>89</v>
       </c>
@@ -3969,7 +3960,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C128" s="18" t="s">
         <v>10</v>
       </c>
@@ -3977,7 +3968,7 @@
       <c r="E128" s="19"/>
       <c r="F128" s="20"/>
     </row>
-    <row r="129" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="C129" s="7"/>
       <c r="D129" s="5" t="s">
         <v>135</v>
@@ -3989,7 +3980,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="11">
         <v>8.1</v>
       </c>
@@ -4003,7 +3994,7 @@
       <c r="E130" s="16"/>
       <c r="F130" s="17"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D131" s="4" t="s">
         <v>1</v>
       </c>
@@ -4014,7 +4005,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="6"/>
       <c r="C132" s="6"/>
       <c r="D132" s="4" t="s">
@@ -4027,7 +4018,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B133" s="6"/>
       <c r="C133" s="6"/>
       <c r="D133" s="4" t="s">
@@ -4040,7 +4031,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="D134" s="5" t="s">
         <v>92</v>
       </c>
@@ -4051,7 +4042,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D135" s="5" t="s">
         <v>49</v>
       </c>
@@ -4062,7 +4053,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D136" s="5" t="s">
         <v>50</v>
       </c>
@@ -4073,7 +4064,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D137" s="5" t="s">
         <v>94</v>
       </c>
@@ -4084,7 +4075,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D138" s="5" t="s">
         <v>95</v>
       </c>
@@ -4095,7 +4086,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D139" s="5" t="s">
         <v>99</v>
       </c>
@@ -4106,7 +4097,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D140" s="5" t="s">
         <v>98</v>
       </c>
@@ -4116,11 +4107,8 @@
       <c r="F140" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="H140" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D141" s="5" t="s">
         <v>96</v>
       </c>
@@ -4131,7 +4119,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D142" s="5" t="s">
         <v>97</v>
       </c>
@@ -4142,7 +4130,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="D143" s="5" t="s">
         <v>93</v>
       </c>
@@ -4153,7 +4141,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C144" s="18" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Propietarios: *CrearCochera *Perfil *Reservas Cliente: *Reservas(faltaMapa) *Confirmar (falta Validacion con horas)
</commit_message>
<xml_diff>
--- a/Consigna/correcciones20162C.xlsx
+++ b/Consigna/correcciones20162C.xlsx
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="148">
   <si>
     <t xml:space="preserve">Página de inicio​ (​/default.aspx​)  </t>
   </si>
@@ -794,6 +794,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -801,15 +810,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2480,29 +2480,29 @@
   <dimension ref="A1:O181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B150" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
+      <selection pane="bottomRight" activeCell="N143" sqref="N143"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="5.75" style="2" customWidth="1"/>
-    <col min="4" max="4" width="84.625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10.25" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="2.625" customWidth="1"/>
-    <col min="8" max="8" width="8.625" customWidth="1"/>
-    <col min="9" max="9" width="4.375" customWidth="1"/>
-    <col min="10" max="10" width="5.375" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="84.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="2.5703125" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" customWidth="1"/>
+    <col min="9" max="9" width="4.42578125" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" customWidth="1"/>
     <col min="11" max="11" width="5" customWidth="1"/>
     <col min="12" max="12" width="3" customWidth="1"/>
-    <col min="13" max="13" width="7.625" customWidth="1"/>
-    <col min="14" max="14" width="7.75" customWidth="1"/>
-    <col min="15" max="15" width="17.625" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="3" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2530,14 +2530,14 @@
       </c>
       <c r="K1">
         <f>COUNTIF(F:F, "B")</f>
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>146</v>
       </c>
       <c r="M1" s="14">
         <f>K1/I1</f>
-        <v>0.98561151079136688</v>
+        <v>1.014388489208633</v>
       </c>
       <c r="N1" s="13" t="s">
         <v>137</v>
@@ -2551,17 +2551,17 @@
       <c r="A2" s="11">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17"/>
-    </row>
-    <row r="3" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="E2" s="19"/>
+      <c r="F2" s="20"/>
+    </row>
+    <row r="3" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -2575,7 +2575,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -2589,7 +2589,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -2605,25 +2605,25 @@
       <c r="A6" s="11">
         <v>1</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="17"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="20"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="17"/>
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2663,7 +2663,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="D11" s="5" t="s">
         <v>12</v>
       </c>
@@ -2687,12 +2687,12 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="20"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D14" s="5" t="s">
@@ -2707,12 +2707,12 @@
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8"/>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="20"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="17"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D16" s="5" t="s">
@@ -2729,8 +2729,11 @@
       <c r="E17" s="5" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D18" s="5" t="s">
         <v>13</v>
       </c>
@@ -2752,12 +2755,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="D20" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>131</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -2767,18 +2773,21 @@
       <c r="E21" s="5" t="s">
         <v>131</v>
       </c>
+      <c r="F21" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>2</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="17"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D23" s="5" t="s">
@@ -2859,12 +2868,12 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="20"/>
-    </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D30" s="17"/>
+    </row>
+    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="D31" s="9" t="s">
         <v>32</v>
       </c>
@@ -2875,7 +2884,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="D32" s="9" t="s">
         <v>34</v>
       </c>
@@ -2890,13 +2899,13 @@
       <c r="A33" s="11">
         <v>3</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="17"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="20"/>
     </row>
     <row r="34" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D34" s="4" t="s">
@@ -2935,7 +2944,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="D37" s="5" t="s">
         <v>27</v>
       </c>
@@ -2959,12 +2968,12 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" s="8"/>
-      <c r="C39" s="18" t="s">
+      <c r="C39" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="20"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="17"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" s="8"/>
@@ -3018,7 +3027,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B44" s="8"/>
       <c r="C44" s="7"/>
       <c r="D44" s="5" t="s">
@@ -3042,7 +3051,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D46" s="5" t="s">
         <v>30</v>
       </c>
@@ -3068,12 +3077,12 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" s="8"/>
-      <c r="C48" s="18" t="s">
+      <c r="C48" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="20"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="17"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
@@ -3116,15 +3125,15 @@
       <c r="A52" s="11">
         <v>4</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B52" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16" t="s">
+      <c r="C52" s="19"/>
+      <c r="D52" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E52" s="16"/>
-      <c r="F52" s="17"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="20"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D53" s="4" t="s">
@@ -3163,7 +3172,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="D56" s="5" t="s">
         <v>41</v>
       </c>
@@ -3175,12 +3184,12 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C57" s="18" t="s">
+      <c r="C57" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="20"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="17"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D58" s="5" t="s">
@@ -3215,21 +3224,24 @@
         <v>139</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="D61" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>131</v>
       </c>
+      <c r="F61" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C62" s="18" t="s">
+      <c r="C62" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D62" s="19"/>
-      <c r="E62" s="19"/>
-      <c r="F62" s="20"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="17"/>
     </row>
     <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D63" s="5" t="s">
@@ -3246,15 +3258,15 @@
       <c r="A64" s="11">
         <v>5</v>
       </c>
-      <c r="B64" s="15" t="s">
+      <c r="B64" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C64" s="16" t="s">
+      <c r="C64" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="17"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="20"/>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D65" s="4" t="s">
@@ -3293,7 +3305,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D68" s="5" t="s">
         <v>11</v>
       </c>
@@ -3305,12 +3317,12 @@
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C69" s="18" t="s">
+      <c r="C69" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D69" s="19"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="20"/>
+      <c r="D69" s="16"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="17"/>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D70" s="5" t="s">
@@ -3521,7 +3533,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D89" s="5" t="s">
         <v>62</v>
       </c>
@@ -3577,12 +3589,12 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C94" s="18" t="s">
+      <c r="C94" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D94" s="19"/>
-      <c r="E94" s="19"/>
-      <c r="F94" s="20"/>
+      <c r="D94" s="16"/>
+      <c r="E94" s="16"/>
+      <c r="F94" s="17"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D95" s="5" t="s">
@@ -3599,15 +3611,15 @@
       <c r="A96" s="11">
         <v>6</v>
       </c>
-      <c r="B96" s="15" t="s">
+      <c r="B96" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C96" s="16" t="s">
+      <c r="C96" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="D96" s="16"/>
-      <c r="E96" s="16"/>
-      <c r="F96" s="17"/>
+      <c r="D96" s="19"/>
+      <c r="E96" s="19"/>
+      <c r="F96" s="20"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D97" s="4" t="s">
@@ -3646,7 +3658,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D100" s="5" t="s">
         <v>11</v>
       </c>
@@ -3658,12 +3670,12 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C101" s="18" t="s">
+      <c r="C101" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D101" s="19"/>
-      <c r="E101" s="19"/>
-      <c r="F101" s="20"/>
+      <c r="D101" s="16"/>
+      <c r="E101" s="16"/>
+      <c r="F101" s="17"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D102" s="5" t="s">
@@ -3722,7 +3734,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="D107" s="5" t="s">
         <v>79</v>
       </c>
@@ -3734,12 +3746,12 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C108" s="18" t="s">
+      <c r="C108" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D108" s="19"/>
-      <c r="E108" s="19"/>
-      <c r="F108" s="20"/>
+      <c r="D108" s="16"/>
+      <c r="E108" s="16"/>
+      <c r="F108" s="17"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D109" s="5" t="s">
@@ -3756,15 +3768,15 @@
       <c r="A110" s="11">
         <v>7</v>
       </c>
-      <c r="B110" s="15" t="s">
+      <c r="B110" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C110" s="16" t="s">
+      <c r="C110" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="D110" s="16"/>
-      <c r="E110" s="16"/>
-      <c r="F110" s="17"/>
+      <c r="D110" s="19"/>
+      <c r="E110" s="19"/>
+      <c r="F110" s="20"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D111" s="4" t="s">
@@ -3803,7 +3815,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="D114" s="5" t="s">
         <v>134</v>
       </c>
@@ -3814,7 +3826,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D115" s="5" t="s">
         <v>88</v>
       </c>
@@ -3826,12 +3838,12 @@
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C116" s="18" t="s">
+      <c r="C116" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D116" s="19"/>
-      <c r="E116" s="19"/>
-      <c r="F116" s="20"/>
+      <c r="D116" s="16"/>
+      <c r="E116" s="16"/>
+      <c r="F116" s="17"/>
     </row>
     <row r="117" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C117" s="7"/>
@@ -3857,7 +3869,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="D119" s="5" t="s">
         <v>83</v>
       </c>
@@ -3869,12 +3881,12 @@
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C120" s="18" t="s">
+      <c r="C120" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D120" s="19"/>
-      <c r="E120" s="19"/>
-      <c r="F120" s="20"/>
+      <c r="D120" s="16"/>
+      <c r="E120" s="16"/>
+      <c r="F120" s="17"/>
     </row>
     <row r="121" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D121" s="5" t="s">
@@ -3891,15 +3903,15 @@
       <c r="A122" s="11">
         <v>8</v>
       </c>
-      <c r="B122" s="15" t="s">
+      <c r="B122" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="C122" s="16" t="s">
+      <c r="C122" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D122" s="16"/>
-      <c r="E122" s="16"/>
-      <c r="F122" s="17"/>
+      <c r="D122" s="19"/>
+      <c r="E122" s="19"/>
+      <c r="F122" s="20"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D123" s="4" t="s">
@@ -3938,7 +3950,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="D126" s="5" t="s">
         <v>90</v>
       </c>
@@ -3961,12 +3973,12 @@
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C128" s="18" t="s">
+      <c r="C128" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D128" s="19"/>
-      <c r="E128" s="19"/>
-      <c r="F128" s="20"/>
+      <c r="D128" s="16"/>
+      <c r="E128" s="16"/>
+      <c r="F128" s="17"/>
     </row>
     <row r="129" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="C129" s="7"/>
@@ -3984,15 +3996,15 @@
       <c r="A130" s="11">
         <v>8.1</v>
       </c>
-      <c r="B130" s="15" t="s">
+      <c r="B130" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="C130" s="16" t="s">
+      <c r="C130" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="D130" s="16"/>
-      <c r="E130" s="16"/>
-      <c r="F130" s="17"/>
+      <c r="D130" s="19"/>
+      <c r="E130" s="19"/>
+      <c r="F130" s="20"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D131" s="4" t="s">
@@ -4031,7 +4043,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="D134" s="5" t="s">
         <v>92</v>
       </c>
@@ -4130,7 +4142,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="143" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="D143" s="5" t="s">
         <v>93</v>
       </c>
@@ -4142,12 +4154,12 @@
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C144" s="18" t="s">
+      <c r="C144" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D144" s="19"/>
-      <c r="E144" s="19"/>
-      <c r="F144" s="20"/>
+      <c r="D144" s="16"/>
+      <c r="E144" s="16"/>
+      <c r="F144" s="17"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D145" s="5" t="s">
@@ -4246,12 +4258,12 @@
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C154" s="18" t="s">
+      <c r="C154" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D154" s="19"/>
-      <c r="E154" s="19"/>
-      <c r="F154" s="20"/>
+      <c r="D154" s="16"/>
+      <c r="E154" s="16"/>
+      <c r="F154" s="17"/>
     </row>
     <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D155" s="5" t="s">
@@ -4279,15 +4291,15 @@
       <c r="A157" s="11">
         <v>9</v>
       </c>
-      <c r="B157" s="15" t="s">
+      <c r="B157" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C157" s="16" t="s">
+      <c r="C157" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="D157" s="16"/>
-      <c r="E157" s="16"/>
-      <c r="F157" s="17"/>
+      <c r="D157" s="19"/>
+      <c r="E157" s="19"/>
+      <c r="F157" s="20"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D158" s="4" t="s">
@@ -4326,7 +4338,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="D161" s="5" t="s">
         <v>108</v>
       </c>
@@ -4387,15 +4399,15 @@
       <c r="A167" s="11">
         <v>10</v>
       </c>
-      <c r="B167" s="15" t="s">
+      <c r="B167" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C167" s="16" t="s">
+      <c r="C167" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="D167" s="16"/>
-      <c r="E167" s="16"/>
-      <c r="F167" s="17"/>
+      <c r="D167" s="19"/>
+      <c r="E167" s="19"/>
+      <c r="F167" s="20"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D168" s="4" t="s">
@@ -4484,15 +4496,15 @@
       <c r="A176" s="11">
         <v>11</v>
       </c>
-      <c r="B176" s="15" t="s">
+      <c r="B176" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="C176" s="16" t="s">
+      <c r="C176" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="D176" s="16"/>
-      <c r="E176" s="16"/>
-      <c r="F176" s="17"/>
+      <c r="D176" s="19"/>
+      <c r="E176" s="19"/>
+      <c r="F176" s="20"/>
     </row>
     <row r="177" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D177" s="5" t="s">
@@ -4551,20 +4563,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C62:F62"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C154:F154"/>
-    <mergeCell ref="B167:F167"/>
-    <mergeCell ref="B176:F176"/>
-    <mergeCell ref="B157:F157"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C69:F69"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="C108:F108"/>
-    <mergeCell ref="C116:F116"/>
-    <mergeCell ref="C120:F120"/>
-    <mergeCell ref="C128:F128"/>
-    <mergeCell ref="C144:F144"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B22:F22"/>
@@ -4581,6 +4579,20 @@
     <mergeCell ref="C39:F39"/>
     <mergeCell ref="C48:F48"/>
     <mergeCell ref="C57:F57"/>
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C154:F154"/>
+    <mergeCell ref="B167:F167"/>
+    <mergeCell ref="B176:F176"/>
+    <mergeCell ref="B157:F157"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C69:F69"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="C108:F108"/>
+    <mergeCell ref="C116:F116"/>
+    <mergeCell ref="C120:F120"/>
+    <mergeCell ref="C128:F128"/>
+    <mergeCell ref="C144:F144"/>
   </mergeCells>
   <conditionalFormatting sqref="E16:E21 E149:E153 E1 E11:E12 E37:E38 E56 E100 E161:E166 E171:E175 E14 E23:E32 E40:E47 E63 E49:E51 E58:E61 E68 E81:E93 E70:E78 E102:E107 E117:E119 E121 E129 E95 E109 E114:E115 E134:E143 E155:E156 E3:E5 E126:E127 E177:E1048576">
     <cfRule type="cellIs" dxfId="134" priority="140" operator="equal">
@@ -5290,7 +5302,7 @@
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
precioTotal que aparezca de entrada, y otras cosas
</commit_message>
<xml_diff>
--- a/Consigna/correcciones20162C.xlsx
+++ b/Consigna/correcciones20162C.xlsx
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="148">
   <si>
     <t xml:space="preserve">Página de inicio​ (​/default.aspx​)  </t>
   </si>
@@ -794,6 +794,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -801,15 +810,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2480,10 +2480,10 @@
   <dimension ref="A1:O181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B150" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N143" sqref="N143"/>
+      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2530,14 +2530,14 @@
       </c>
       <c r="K1">
         <f>COUNTIF(F:F, "B")</f>
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>146</v>
       </c>
       <c r="M1" s="14">
         <f>K1/I1</f>
-        <v>1.014388489208633</v>
+        <v>1.064748201438849</v>
       </c>
       <c r="N1" s="13" t="s">
         <v>137</v>
@@ -2551,15 +2551,15 @@
       <c r="A2" s="11">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="3" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -2599,31 +2599,33 @@
       <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="9"/>
+      <c r="F5" s="9" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>1</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="17"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="20"/>
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2687,12 +2689,12 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="20"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D14" s="5" t="s">
@@ -2707,12 +2709,12 @@
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8"/>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="20"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D16" s="5" t="s">
@@ -2781,13 +2783,13 @@
       <c r="A22" s="11">
         <v>2</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="20"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="17"/>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D23" s="5" t="s">
@@ -2868,10 +2870,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="17"/>
+      <c r="D30" s="20"/>
     </row>
     <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="D31" s="9" t="s">
@@ -2899,13 +2901,13 @@
       <c r="A33" s="11">
         <v>3</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="20"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="17"/>
     </row>
     <row r="34" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D34" s="4" t="s">
@@ -2968,12 +2970,12 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" s="8"/>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="17"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="20"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" s="8"/>
@@ -3077,12 +3079,12 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" s="8"/>
-      <c r="C48" s="15" t="s">
+      <c r="C48" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D48" s="16"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="17"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="20"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
@@ -3125,15 +3127,15 @@
       <c r="A52" s="11">
         <v>4</v>
       </c>
-      <c r="B52" s="18" t="s">
+      <c r="B52" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19" t="s">
+      <c r="C52" s="16"/>
+      <c r="D52" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E52" s="19"/>
-      <c r="F52" s="20"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="17"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D53" s="4" t="s">
@@ -3184,12 +3186,12 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C57" s="15" t="s">
+      <c r="C57" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D57" s="16"/>
-      <c r="E57" s="16"/>
-      <c r="F57" s="17"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="20"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D58" s="5" t="s">
@@ -3236,12 +3238,12 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C62" s="15" t="s">
+      <c r="C62" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="17"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="20"/>
     </row>
     <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D63" s="5" t="s">
@@ -3258,15 +3260,15 @@
       <c r="A64" s="11">
         <v>5</v>
       </c>
-      <c r="B64" s="18" t="s">
+      <c r="B64" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C64" s="19" t="s">
+      <c r="C64" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D64" s="19"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="20"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="17"/>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D65" s="4" t="s">
@@ -3317,12 +3319,12 @@
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C69" s="15" t="s">
+      <c r="C69" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D69" s="16"/>
-      <c r="E69" s="16"/>
-      <c r="F69" s="17"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="20"/>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D70" s="5" t="s">
@@ -3589,12 +3591,12 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C94" s="15" t="s">
+      <c r="C94" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D94" s="16"/>
-      <c r="E94" s="16"/>
-      <c r="F94" s="17"/>
+      <c r="D94" s="19"/>
+      <c r="E94" s="19"/>
+      <c r="F94" s="20"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D95" s="5" t="s">
@@ -3611,15 +3613,15 @@
       <c r="A96" s="11">
         <v>6</v>
       </c>
-      <c r="B96" s="18" t="s">
+      <c r="B96" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C96" s="19" t="s">
+      <c r="C96" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="D96" s="19"/>
-      <c r="E96" s="19"/>
-      <c r="F96" s="20"/>
+      <c r="D96" s="16"/>
+      <c r="E96" s="16"/>
+      <c r="F96" s="17"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D97" s="4" t="s">
@@ -3670,12 +3672,12 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C101" s="15" t="s">
+      <c r="C101" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D101" s="16"/>
-      <c r="E101" s="16"/>
-      <c r="F101" s="17"/>
+      <c r="D101" s="19"/>
+      <c r="E101" s="19"/>
+      <c r="F101" s="20"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D102" s="5" t="s">
@@ -3746,12 +3748,12 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C108" s="15" t="s">
+      <c r="C108" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D108" s="16"/>
-      <c r="E108" s="16"/>
-      <c r="F108" s="17"/>
+      <c r="D108" s="19"/>
+      <c r="E108" s="19"/>
+      <c r="F108" s="20"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D109" s="5" t="s">
@@ -3768,15 +3770,15 @@
       <c r="A110" s="11">
         <v>7</v>
       </c>
-      <c r="B110" s="18" t="s">
+      <c r="B110" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C110" s="19" t="s">
+      <c r="C110" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="D110" s="19"/>
-      <c r="E110" s="19"/>
-      <c r="F110" s="20"/>
+      <c r="D110" s="16"/>
+      <c r="E110" s="16"/>
+      <c r="F110" s="17"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D111" s="4" t="s">
@@ -3838,12 +3840,12 @@
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C116" s="15" t="s">
+      <c r="C116" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D116" s="16"/>
-      <c r="E116" s="16"/>
-      <c r="F116" s="17"/>
+      <c r="D116" s="19"/>
+      <c r="E116" s="19"/>
+      <c r="F116" s="20"/>
     </row>
     <row r="117" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C117" s="7"/>
@@ -3881,12 +3883,12 @@
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C120" s="15" t="s">
+      <c r="C120" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D120" s="16"/>
-      <c r="E120" s="16"/>
-      <c r="F120" s="17"/>
+      <c r="D120" s="19"/>
+      <c r="E120" s="19"/>
+      <c r="F120" s="20"/>
     </row>
     <row r="121" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D121" s="5" t="s">
@@ -3903,15 +3905,15 @@
       <c r="A122" s="11">
         <v>8</v>
       </c>
-      <c r="B122" s="18" t="s">
+      <c r="B122" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="C122" s="19" t="s">
+      <c r="C122" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="D122" s="19"/>
-      <c r="E122" s="19"/>
-      <c r="F122" s="20"/>
+      <c r="D122" s="16"/>
+      <c r="E122" s="16"/>
+      <c r="F122" s="17"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D123" s="4" t="s">
@@ -3973,12 +3975,12 @@
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C128" s="15" t="s">
+      <c r="C128" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D128" s="16"/>
-      <c r="E128" s="16"/>
-      <c r="F128" s="17"/>
+      <c r="D128" s="19"/>
+      <c r="E128" s="19"/>
+      <c r="F128" s="20"/>
     </row>
     <row r="129" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="C129" s="7"/>
@@ -3996,15 +3998,15 @@
       <c r="A130" s="11">
         <v>8.1</v>
       </c>
-      <c r="B130" s="18" t="s">
+      <c r="B130" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="C130" s="19" t="s">
+      <c r="C130" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="D130" s="19"/>
-      <c r="E130" s="19"/>
-      <c r="F130" s="20"/>
+      <c r="D130" s="16"/>
+      <c r="E130" s="16"/>
+      <c r="F130" s="17"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D131" s="4" t="s">
@@ -4154,12 +4156,12 @@
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C144" s="15" t="s">
+      <c r="C144" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D144" s="16"/>
-      <c r="E144" s="16"/>
-      <c r="F144" s="17"/>
+      <c r="D144" s="19"/>
+      <c r="E144" s="19"/>
+      <c r="F144" s="20"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D145" s="5" t="s">
@@ -4256,14 +4258,17 @@
       <c r="E153" s="5" t="s">
         <v>131</v>
       </c>
+      <c r="F153" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C154" s="15" t="s">
+      <c r="C154" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D154" s="16"/>
-      <c r="E154" s="16"/>
-      <c r="F154" s="17"/>
+      <c r="D154" s="19"/>
+      <c r="E154" s="19"/>
+      <c r="F154" s="20"/>
     </row>
     <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D155" s="5" t="s">
@@ -4291,15 +4296,15 @@
       <c r="A157" s="11">
         <v>9</v>
       </c>
-      <c r="B157" s="18" t="s">
+      <c r="B157" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="C157" s="19" t="s">
+      <c r="C157" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="D157" s="19"/>
-      <c r="E157" s="19"/>
-      <c r="F157" s="20"/>
+      <c r="D157" s="16"/>
+      <c r="E157" s="16"/>
+      <c r="F157" s="17"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D158" s="4" t="s">
@@ -4356,6 +4361,9 @@
       <c r="E162" s="5" t="s">
         <v>131</v>
       </c>
+      <c r="F162" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D163" s="5" t="s">
@@ -4394,20 +4402,23 @@
       <c r="E166" s="5" t="s">
         <v>131</v>
       </c>
+      <c r="F166" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="11">
         <v>10</v>
       </c>
-      <c r="B167" s="18" t="s">
+      <c r="B167" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C167" s="19" t="s">
+      <c r="C167" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="D167" s="19"/>
-      <c r="E167" s="19"/>
-      <c r="F167" s="20"/>
+      <c r="D167" s="16"/>
+      <c r="E167" s="16"/>
+      <c r="F167" s="17"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D168" s="4" t="s">
@@ -4453,6 +4464,9 @@
       <c r="E171" s="5" t="s">
         <v>131</v>
       </c>
+      <c r="F171" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D172" s="5" t="s">
@@ -4461,6 +4475,9 @@
       <c r="E172" s="5" t="s">
         <v>131</v>
       </c>
+      <c r="F172" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="173" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D173" s="5" t="s">
@@ -4491,20 +4508,23 @@
       <c r="E175" s="5" t="s">
         <v>131</v>
       </c>
+      <c r="F175" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="11">
         <v>11</v>
       </c>
-      <c r="B176" s="18" t="s">
+      <c r="B176" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="C176" s="19" t="s">
+      <c r="C176" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="D176" s="19"/>
-      <c r="E176" s="19"/>
-      <c r="F176" s="20"/>
+      <c r="D176" s="16"/>
+      <c r="E176" s="16"/>
+      <c r="F176" s="17"/>
     </row>
     <row r="177" spans="4:6" ht="30" x14ac:dyDescent="0.25">
       <c r="D177" s="5" t="s">
@@ -4563,6 +4583,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C154:F154"/>
+    <mergeCell ref="B167:F167"/>
+    <mergeCell ref="B176:F176"/>
+    <mergeCell ref="B157:F157"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C69:F69"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="C108:F108"/>
+    <mergeCell ref="C116:F116"/>
+    <mergeCell ref="C120:F120"/>
+    <mergeCell ref="C128:F128"/>
+    <mergeCell ref="C144:F144"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B22:F22"/>
@@ -4579,20 +4613,6 @@
     <mergeCell ref="C39:F39"/>
     <mergeCell ref="C48:F48"/>
     <mergeCell ref="C57:F57"/>
-    <mergeCell ref="C62:F62"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C154:F154"/>
-    <mergeCell ref="B167:F167"/>
-    <mergeCell ref="B176:F176"/>
-    <mergeCell ref="B157:F157"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C69:F69"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="C108:F108"/>
-    <mergeCell ref="C116:F116"/>
-    <mergeCell ref="C120:F120"/>
-    <mergeCell ref="C128:F128"/>
-    <mergeCell ref="C144:F144"/>
   </mergeCells>
   <conditionalFormatting sqref="E16:E21 E149:E153 E1 E11:E12 E37:E38 E56 E100 E161:E166 E171:E175 E14 E23:E32 E40:E47 E63 E49:E51 E58:E61 E68 E81:E93 E70:E78 E102:E107 E117:E119 E121 E129 E95 E109 E114:E115 E134:E143 E155:E156 E3:E5 E126:E127 E177:E1048576">
     <cfRule type="cellIs" dxfId="134" priority="140" operator="equal">

</xml_diff>